<commit_message>
Pad shared memory arrays; Coalesce global memory accesses; Add .clang-format; Format code
</commit_message>
<xml_diff>
--- a/recursivefiltering.xlsx
+++ b/recursivefiltering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\recursivefilter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE0EF01-3888-4745-852F-095616100712}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78EC254-9173-4D2C-94F8-5EE62826BDED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{678362C0-2759-4A65-8D7C-538BF80720F9}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA7F144-7574-43E2-A102-27BDE7BCC9E2}">
   <dimension ref="A1:AP63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="AG47" sqref="AG47"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -515,7 +515,7 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="B2" s="13">
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="D2" s="14">
         <v>1</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="B3" s="13">
-        <v>0.54600000000000004</v>
+        <v>1</v>
       </c>
       <c r="D3" s="14">
         <v>2</v>
@@ -761,7 +761,7 @@
     <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D9" s="2">
         <f t="shared" ref="D9:I14" si="0">$B$2*D2+$B$3*D8</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
@@ -773,11 +773,11 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="0"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
@@ -785,7 +785,7 @@
       </c>
       <c r="K9" s="9">
         <f>$B$2*D2+$B$3*K8</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="L9" s="9">
         <f t="shared" ref="L9:P9" si="1">$B$2*E2+$B$3*L8</f>
@@ -797,11 +797,11 @@
       </c>
       <c r="N9" s="9">
         <f t="shared" si="1"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="O9" s="9">
         <f t="shared" si="1"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="P9" s="9">
         <f t="shared" si="1"/>
@@ -809,11 +809,11 @@
       </c>
       <c r="R9" s="3">
         <f t="shared" ref="R9:S14" si="2">$B$2*K9+$B$3*Q9</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="S9" s="12">
         <f t="shared" si="2"/>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="T9" s="3">
         <f t="shared" ref="T9:T14" si="3">$B$2*M9+$B$3*Q9</f>
@@ -821,69 +821,69 @@
       </c>
       <c r="U9" s="12">
         <f t="shared" ref="U9:U14" si="4">$B$2*N9+$B$3*T9</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="V9" s="3">
         <f>$B$2*O9+$B$3*Q9</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="W9" s="12">
         <f t="shared" ref="W9:W14" si="5">$B$2*P9+$B$3*V9</f>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="AD9" s="1" t="str">
         <f>K10 &amp; "f,"</f>
-        <v>4.386758f,</v>
+        <v>3f,</v>
       </c>
       <c r="AE9" s="1" t="str">
         <f>L10 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <v>1f,</v>
       </c>
       <c r="AF9" s="1" t="str">
         <f>M10 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <v>1f,</v>
       </c>
       <c r="AG9" s="1" t="str">
         <f>N10 &amp; "f,"</f>
-        <v>2.663758f,</v>
+        <v>2f,</v>
       </c>
       <c r="AH9" s="1" t="str">
         <f>O10 &amp; "f,"</f>
-        <v>4.386758f,</v>
+        <v>3f,</v>
       </c>
       <c r="AJ9" s="1" t="str">
         <f>S9 &amp; "f,"</f>
-        <v>1.620926034f,</v>
+        <v>1f,</v>
       </c>
       <c r="AK9" s="1" t="str">
         <f>U9 &amp; "f,"</f>
-        <v>2.968729f,</v>
+        <v>1f,</v>
       </c>
       <c r="AL9" s="1" t="str">
         <f>W9 &amp; "f,"</f>
-        <v>1.620926034f,</v>
+        <v>1f,</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>2.6637580000000001</v>
+        <v>2</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="0"/>
@@ -891,23 +891,23 @@
       </c>
       <c r="K10" s="10">
         <f>$B$2*D3+$B$3*K9</f>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="L10" s="10">
         <f t="shared" ref="L10:P10" si="6">$B$2*E3+$B$3*L9</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="M10" s="10">
         <f t="shared" si="6"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="N10" s="10">
         <f t="shared" si="6"/>
-        <v>2.6637580000000001</v>
+        <v>2</v>
       </c>
       <c r="O10" s="10">
         <f t="shared" si="6"/>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="P10" s="10">
         <f t="shared" si="6"/>
@@ -915,81 +915,81 @@
       </c>
       <c r="R10" s="3">
         <f t="shared" si="2"/>
-        <v>7.5583840340000013</v>
+        <v>3</v>
       </c>
       <c r="S10" s="12">
         <f t="shared" si="2"/>
-        <v>7.0956066825640018</v>
+        <v>4</v>
       </c>
       <c r="T10" s="3">
         <f t="shared" si="3"/>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="U10" s="12">
         <f t="shared" si="4"/>
-        <v>6.2105810680000006</v>
+        <v>3</v>
       </c>
       <c r="V10" s="3">
         <f t="shared" ref="V10:V14" si="7">$B$2*O10+$B$3*Q10</f>
-        <v>7.5583840340000013</v>
+        <v>3</v>
       </c>
       <c r="W10" s="12">
         <f t="shared" si="5"/>
-        <v>4.1268776825640012</v>
+        <v>3</v>
       </c>
       <c r="AD10" s="1" t="str">
         <f>K12 &amp; "f,"</f>
-        <v>2.663758f,</v>
+        <v>2f,</v>
       </c>
       <c r="AE10" s="1" t="str">
         <f>L12 &amp; "f,"</f>
-        <v>3.604516f,</v>
+        <v>3f,</v>
       </c>
       <c r="AF10" s="1" t="str">
         <f>M12 &amp; "f,"</f>
-        <v>0.940758f,</v>
+        <v>1f,</v>
       </c>
       <c r="AG10" s="1" t="str">
         <f>N12 &amp; "f,"</f>
-        <v>3.604516f,</v>
+        <v>3f,</v>
       </c>
       <c r="AH10" s="1" t="str">
         <f>O12 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <v>1f,</v>
       </c>
       <c r="AJ10" s="1" t="str">
         <f>S10 &amp; "f,"</f>
-        <v>7.095606682564f,</v>
+        <v>4f,</v>
       </c>
       <c r="AK10" s="1" t="str">
         <f>U10 &amp; "f,"</f>
-        <v>6.210581068f,</v>
+        <v>3f,</v>
       </c>
       <c r="AL10" s="1" t="str">
         <f>W10 &amp; "f,"</f>
-        <v>4.126877682564f,</v>
+        <v>3f,</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>4.1181698680000007</v>
+        <v>4</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>2.6637580000000001</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>4.9004118680000008</v>
+        <v>4</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>2.3951698680000004</v>
+        <v>3</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="0"/>
@@ -997,19 +997,19 @@
       </c>
       <c r="K11" s="9">
         <f>$B$2*D4+$B$3*K8</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="L11" s="9">
         <f t="shared" ref="L11:P11" si="8">$B$2*E4+$B$3*L8</f>
-        <v>3.4460000000000002</v>
+        <v>2</v>
       </c>
       <c r="M11" s="9">
         <f t="shared" si="8"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="N11" s="9">
         <f t="shared" si="8"/>
-        <v>3.4460000000000002</v>
+        <v>2</v>
       </c>
       <c r="O11" s="9">
         <f t="shared" si="8"/>
@@ -1021,19 +1021,19 @@
       </c>
       <c r="R11" s="3">
         <f t="shared" si="2"/>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="S11" s="12">
         <f t="shared" si="2"/>
-        <v>7.5583840340000004</v>
+        <v>3</v>
       </c>
       <c r="T11" s="3">
         <f t="shared" si="3"/>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="U11" s="12">
         <f t="shared" si="4"/>
-        <v>7.5583840340000004</v>
+        <v>3</v>
       </c>
       <c r="V11" s="3">
         <f t="shared" si="7"/>
@@ -1049,27 +1049,27 @@
       </c>
       <c r="AE11" s="1" t="str">
         <f>L14 &amp; "f,"</f>
-        <v>0.940758f,</v>
+        <v>1f,</v>
       </c>
       <c r="AF11" s="1" t="str">
         <f>M14 &amp; "f,"</f>
-        <v>1.881516f,</v>
+        <v>2f,</v>
       </c>
       <c r="AG11" s="1" t="str">
         <f>N14 &amp; "f,"</f>
-        <v>0.940758f,</v>
+        <v>1f,</v>
       </c>
       <c r="AH11" s="1" t="str">
         <f>O14 &amp; "f,"</f>
-        <v>1.881516f,</v>
+        <v>2f,</v>
       </c>
       <c r="AJ11" s="1" t="str">
         <f>S11 &amp; "f,"</f>
-        <v>7.558384034f,</v>
+        <v>3f,</v>
       </c>
       <c r="AK11" s="1" t="str">
         <f>U11 &amp; "f,"</f>
-        <v>7.558384034f,</v>
+        <v>3f,</v>
       </c>
       <c r="AL11" s="1" t="str">
         <f>W11 &amp; "f,"</f>
@@ -1079,23 +1079,23 @@
     <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>3.9715207479280004</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>4.1181698680000007</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>1.4544118680000002</v>
+        <v>2</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>4.3986248799280006</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>3.0307627479280006</v>
+        <v>4</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="0"/>
@@ -1103,23 +1103,23 @@
       </c>
       <c r="K12" s="10">
         <f t="shared" ref="K12" si="9">$B$2*D5+$B$3*K11</f>
-        <v>2.6637580000000001</v>
+        <v>2</v>
       </c>
       <c r="L12" s="10">
         <f t="shared" ref="L12" si="10">$B$2*E5+$B$3*L11</f>
-        <v>3.6045160000000003</v>
+        <v>3</v>
       </c>
       <c r="M12" s="10">
         <f t="shared" ref="M12" si="11">$B$2*F5+$B$3*M11</f>
-        <v>0.94075800000000009</v>
+        <v>1</v>
       </c>
       <c r="N12" s="10">
         <f t="shared" ref="N12" si="12">$B$2*G5+$B$3*N11</f>
-        <v>3.6045160000000003</v>
+        <v>3</v>
       </c>
       <c r="O12" s="10">
         <f t="shared" ref="O12" si="13">$B$2*H5+$B$3*O11</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="P12" s="10">
         <f t="shared" ref="P12" si="14">$B$2*I5+$B$3*P11</f>
@@ -1127,61 +1127,61 @@
       </c>
       <c r="R12" s="3">
         <f t="shared" si="2"/>
-        <v>4.5896550340000006</v>
+        <v>2</v>
       </c>
       <c r="S12" s="12">
         <f t="shared" si="2"/>
-        <v>8.7165327165640001</v>
+        <v>5</v>
       </c>
       <c r="T12" s="3">
         <f t="shared" si="3"/>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="U12" s="12">
         <f t="shared" si="4"/>
-        <v>7.095606682564001</v>
+        <v>4</v>
       </c>
       <c r="V12" s="3">
         <f t="shared" si="7"/>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="W12" s="12">
         <f t="shared" si="5"/>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="AJ12" s="1" t="str">
         <f>S12 &amp; "f,"</f>
-        <v>8.716532716564f,</v>
+        <v>5f,</v>
       </c>
       <c r="AK12" s="1" t="str">
         <f>U12 &amp; "f,"</f>
-        <v>7.095606682564f,</v>
+        <v>4f,</v>
       </c>
       <c r="AL12" s="1" t="str">
         <f>W12 &amp; "f,"</f>
-        <v>1.620926034f,</v>
+        <v>1f,</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>2.1684503283686882</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>3.9715207479280004</v>
+        <v>5</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>4.240108879928</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>4.1246491844406883</v>
+        <v>6</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="0"/>
-        <v>5.1007964603686888</v>
+        <v>6</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="0"/>
@@ -1193,19 +1193,19 @@
       </c>
       <c r="L13" s="9">
         <f t="shared" ref="L13:P13" si="15">$B$2*E6+$B$3*L8</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="M13" s="9">
         <f t="shared" si="15"/>
-        <v>3.4460000000000002</v>
+        <v>2</v>
       </c>
       <c r="N13" s="9">
         <f t="shared" si="15"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="O13" s="9">
         <f t="shared" si="15"/>
-        <v>3.4460000000000002</v>
+        <v>2</v>
       </c>
       <c r="P13" s="9">
         <f t="shared" si="15"/>
@@ -1217,57 +1217,57 @@
       </c>
       <c r="S13" s="12">
         <f t="shared" si="2"/>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="T13" s="3">
         <f t="shared" si="3"/>
-        <v>5.9374580000000003</v>
+        <v>2</v>
       </c>
       <c r="U13" s="12">
         <f t="shared" si="4"/>
-        <v>6.2105810680000006</v>
+        <v>3</v>
       </c>
       <c r="V13" s="3">
         <f t="shared" si="7"/>
-        <v>5.9374580000000003</v>
+        <v>2</v>
       </c>
       <c r="W13" s="12">
         <f t="shared" si="5"/>
-        <v>3.2418520680000005</v>
+        <v>2</v>
       </c>
       <c r="AJ13" s="1" t="str">
         <f>S13 &amp; "f,"</f>
-        <v>2.968729f,</v>
+        <v>1f,</v>
       </c>
       <c r="AK13" s="1" t="str">
         <f>U13 &amp; "f,"</f>
-        <v>6.210581068f,</v>
+        <v>3f,</v>
       </c>
       <c r="AL13" s="1" t="str">
         <f>W13 &amp; "f,"</f>
-        <v>3.241852068f,</v>
+        <v>2f,</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>1.1839738792893038</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>2.1684503283686882</v>
+        <v>5</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>2.3150994484406882</v>
+        <v>4</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>2.2520584547046161</v>
+        <v>6</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="0"/>
-        <v>2.7850348673613041</v>
+        <v>6</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="0"/>
@@ -1279,19 +1279,19 @@
       </c>
       <c r="L14" s="10">
         <f t="shared" ref="L14" si="17">$B$2*E7+$B$3*L13</f>
-        <v>0.94075800000000009</v>
+        <v>1</v>
       </c>
       <c r="M14" s="10">
         <f t="shared" ref="M14" si="18">$B$2*F7+$B$3*M13</f>
-        <v>1.8815160000000002</v>
+        <v>2</v>
       </c>
       <c r="N14" s="10">
         <f t="shared" ref="N14" si="19">$B$2*G7+$B$3*N13</f>
-        <v>0.94075800000000009</v>
+        <v>1</v>
       </c>
       <c r="O14" s="10">
         <f t="shared" ref="O14" si="20">$B$2*H7+$B$3*O13</f>
-        <v>1.8815160000000002</v>
+        <v>2</v>
       </c>
       <c r="P14" s="10">
         <f t="shared" ref="P14" si="21">$B$2*I7+$B$3*P13</f>
@@ -1303,69 +1303,69 @@
       </c>
       <c r="S14" s="12">
         <f t="shared" si="2"/>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="T14" s="3">
         <f t="shared" si="3"/>
-        <v>3.2418520680000005</v>
+        <v>2</v>
       </c>
       <c r="U14" s="12">
         <f t="shared" si="4"/>
-        <v>3.3909772631280006</v>
+        <v>3</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="7"/>
-        <v>3.2418520680000005</v>
+        <v>2</v>
       </c>
       <c r="W14" s="12">
         <f t="shared" si="5"/>
-        <v>1.7700512291280004</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D16" s="2">
         <f>$B$2*D9+$B$3*C16</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" ref="E16:I16" si="22">$B$2*E9+$B$3*D16</f>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="22"/>
-        <v>0.8850256145640002</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="22"/>
-        <v>3.4519529855519444</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="22"/>
-        <v>4.8534953301113619</v>
+        <v>3</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="22"/>
-        <v>2.6500084502408039</v>
+        <v>3</v>
       </c>
       <c r="K16" s="11">
         <f>K10+$B$3*$B$3*K8</f>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="L16" s="11">
         <f t="shared" ref="L16:P16" si="23">L10+$B$3*$B$3*L8</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="M16" s="11">
         <f t="shared" si="23"/>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="N16" s="11">
         <f t="shared" si="23"/>
-        <v>2.6637580000000001</v>
+        <v>2</v>
       </c>
       <c r="O16" s="11">
         <f t="shared" si="23"/>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="P16" s="11">
         <f t="shared" si="23"/>
@@ -1373,491 +1373,491 @@
       </c>
       <c r="R16" s="4">
         <f>$B$2*K16+$B$3*Q16</f>
-        <v>7.5583840340000013</v>
+        <v>3</v>
       </c>
       <c r="S16" s="5">
         <f>$B$2*L16+$B$3*R16</f>
-        <v>7.0956066825640018</v>
+        <v>4</v>
       </c>
       <c r="T16" s="4">
         <f>$B$2*M16+$B$3*Q16</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="U16" s="5">
         <f>$B$2*N16+$B$3*T16</f>
-        <v>6.2105810680000006</v>
+        <v>3</v>
       </c>
       <c r="V16" s="4">
         <f>$B$2*O16+$B$3*Q16</f>
-        <v>7.5583840340000013</v>
+        <v>3</v>
       </c>
       <c r="W16" s="5">
         <f>$B$2*P16+$B$3*V16</f>
-        <v>4.1268776825640012</v>
+        <v>3</v>
       </c>
       <c r="Y16" s="6">
         <f>S9+$B$3*$B$3*X16+$B$3*S15</f>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="Z16" s="6">
         <f>U9+$B$3*$B$3*Y16+$B$3*U15</f>
-        <v>3.4519529855519444</v>
+        <v>2</v>
       </c>
       <c r="AA16" s="6">
         <f>W9+$B$3*$B$3*Z16+$B$3*W15</f>
-        <v>2.6500084502408039</v>
+        <v>3</v>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1" t="str">
         <f>K16 &amp; "f,"</f>
-        <v>4.386758f,</v>
+        <v>3f,</v>
       </c>
       <c r="AE16" s="1" t="str">
         <f t="shared" ref="AE16:AE18" si="24">L16 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <v>1f,</v>
       </c>
       <c r="AF16" s="1" t="str">
         <f t="shared" ref="AF16:AF18" si="25">M16 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <v>1f,</v>
       </c>
       <c r="AG16" s="1" t="str">
         <f t="shared" ref="AG16:AG18" si="26">N16 &amp; "f,"</f>
-        <v>2.663758f,</v>
+        <v>2f,</v>
       </c>
       <c r="AH16" s="1" t="str">
         <f t="shared" ref="AH16:AH18" si="27">O16 &amp; "f,"</f>
-        <v>4.386758f,</v>
+        <v>3f,</v>
       </c>
       <c r="AJ16" s="1" t="str">
         <f>S16 &amp; "f,"</f>
-        <v>7.095606682564f,</v>
+        <v>4f,</v>
       </c>
       <c r="AK16" s="1" t="str">
         <f>U16 &amp; "f,"</f>
-        <v>6.210581068f,</v>
+        <v>3f,</v>
       </c>
       <c r="AL16" s="1" t="str">
         <f>W16 &amp; "f,"</f>
-        <v>4.126877682564f,</v>
+        <v>3f,</v>
       </c>
       <c r="AN16" s="1" t="str">
-        <f>Y16 &amp; "f,"</f>
-        <v>1.620926034f,</v>
+        <f t="shared" ref="AN16:AP20" si="28">Y16 &amp; "f,"</f>
+        <v>1f,</v>
       </c>
       <c r="AO16" s="1" t="str">
-        <f>Z16 &amp; "f,"</f>
-        <v>3.45195298555194f,</v>
+        <f t="shared" si="28"/>
+        <v>2f,</v>
       </c>
       <c r="AP16" s="1" t="str">
-        <f>AA16 &amp; "f,"</f>
-        <v>2.6500084502408f,</v>
+        <f t="shared" si="28"/>
+        <v>3f,</v>
       </c>
     </row>
     <row r="17" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D17" s="2">
-        <f t="shared" ref="D17:I17" si="28">$B$2*D10+$B$3*C17</f>
-        <v>7.5583840340000013</v>
+        <f t="shared" ref="D17:I17" si="29">$B$2*D10+$B$3*C17</f>
+        <v>3</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="28"/>
-        <v>7.0956066825640018</v>
+        <f t="shared" si="29"/>
+        <v>4</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="28"/>
-        <v>6.842930248679945</v>
+        <f t="shared" si="29"/>
+        <v>5</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="28"/>
-        <v>8.3258949497792507</v>
+        <f t="shared" si="29"/>
+        <v>7</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="28"/>
-        <v>12.104322676579471</v>
+        <f t="shared" si="29"/>
+        <v>10</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="28"/>
-        <v>6.6089601814123915</v>
+        <f t="shared" si="29"/>
+        <v>10</v>
       </c>
       <c r="K17" s="11">
         <f>K12+$B$3*$B$3*K16</f>
-        <v>3.9715207479280004</v>
+        <v>5</v>
       </c>
       <c r="L17" s="11">
-        <f t="shared" ref="L17:P17" si="29">L12+$B$3*$B$3*L16</f>
-        <v>4.1181698680000007</v>
+        <f t="shared" ref="L17:P17" si="30">L12+$B$3*$B$3*L16</f>
+        <v>4</v>
       </c>
       <c r="M17" s="11">
-        <f t="shared" si="29"/>
-        <v>1.4544118680000002</v>
+        <f t="shared" si="30"/>
+        <v>2</v>
       </c>
       <c r="N17" s="11">
-        <f t="shared" si="29"/>
-        <v>4.3986248799280006</v>
+        <f t="shared" si="30"/>
+        <v>5</v>
       </c>
       <c r="O17" s="11">
-        <f t="shared" si="29"/>
-        <v>3.0307627479280006</v>
+        <f t="shared" si="30"/>
+        <v>4</v>
       </c>
       <c r="P17" s="11">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R17" s="4">
-        <f t="shared" ref="R17:S17" si="30">$B$2*K17+$B$3*Q17</f>
-        <v>6.842930248679945</v>
+        <f t="shared" ref="R17:S17" si="31">$B$2*K17+$B$3*Q17</f>
+        <v>5</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" si="30"/>
-        <v>10.831846598343251</v>
+        <f t="shared" si="31"/>
+        <v>9</v>
       </c>
       <c r="T17" s="4">
-        <f t="shared" ref="T17:T18" si="31">$B$2*M17+$B$3*Q17</f>
-        <v>2.5059516485640003</v>
+        <f t="shared" ref="T17:T18" si="32">$B$2*M17+$B$3*Q17</f>
+        <v>2</v>
       </c>
       <c r="U17" s="5">
-        <f t="shared" ref="U17:U18" si="32">$B$2*N17+$B$3*T17</f>
-        <v>8.9470802682318897</v>
+        <f t="shared" ref="U17:U18" si="33">$B$2*N17+$B$3*T17</f>
+        <v>7</v>
       </c>
       <c r="V17" s="4">
-        <f t="shared" ref="V17:V18" si="33">$B$2*O17+$B$3*Q17</f>
-        <v>5.222004214679945</v>
+        <f t="shared" ref="V17:V18" si="34">$B$2*O17+$B$3*Q17</f>
+        <v>4</v>
       </c>
       <c r="W17" s="5">
-        <f t="shared" ref="W17:W18" si="34">$B$2*P17+$B$3*V17</f>
-        <v>2.8512143012152502</v>
+        <f t="shared" ref="W17:W18" si="35">$B$2*P17+$B$3*V17</f>
+        <v>4</v>
       </c>
       <c r="Y17" s="6">
         <f>S10+$B$3*$B$3*X17+$B$3*$B$3*S15</f>
-        <v>7.0956066825640018</v>
+        <v>4</v>
       </c>
       <c r="Z17" s="6">
         <f>U10+$B$3*$B$3*Y17+$B$3*U15</f>
-        <v>8.3258949497792507</v>
+        <v>7</v>
       </c>
       <c r="AA17" s="6">
         <f>W10+$B$3*$B$3*Z17+$B$3*W15</f>
-        <v>6.6089601814123924</v>
+        <v>10</v>
       </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1" t="str">
-        <f t="shared" ref="AD17:AD18" si="35">K17 &amp; "f,"</f>
-        <v>3.971520747928f,</v>
+        <f t="shared" ref="AD17:AD18" si="36">K17 &amp; "f,"</f>
+        <v>5f,</v>
       </c>
       <c r="AE17" s="1" t="str">
         <f t="shared" si="24"/>
-        <v>4.118169868f,</v>
+        <v>4f,</v>
       </c>
       <c r="AF17" s="1" t="str">
         <f t="shared" si="25"/>
-        <v>1.454411868f,</v>
+        <v>2f,</v>
       </c>
       <c r="AG17" s="1" t="str">
         <f t="shared" si="26"/>
-        <v>4.398624879928f,</v>
+        <v>5f,</v>
       </c>
       <c r="AH17" s="1" t="str">
         <f t="shared" si="27"/>
-        <v>3.030762747928f,</v>
+        <v>4f,</v>
       </c>
       <c r="AJ17" s="1" t="str">
-        <f t="shared" ref="AJ17:AJ18" si="36">S17 &amp; "f,"</f>
-        <v>10.8318465983433f,</v>
+        <f t="shared" ref="AJ17:AJ18" si="37">S17 &amp; "f,"</f>
+        <v>9f,</v>
       </c>
       <c r="AK17" s="1" t="str">
-        <f t="shared" ref="AK17:AK18" si="37">U17 &amp; "f,"</f>
-        <v>8.94708026823189f,</v>
+        <f t="shared" ref="AK17:AK18" si="38">U17 &amp; "f,"</f>
+        <v>7f,</v>
       </c>
       <c r="AL17" s="1" t="str">
-        <f t="shared" ref="AL17:AL18" si="38">W17 &amp; "f,"</f>
-        <v>2.85121430121525f,</v>
+        <f t="shared" ref="AL17:AL18" si="39">W17 &amp; "f,"</f>
+        <v>4f,</v>
       </c>
       <c r="AN17" s="1" t="str">
-        <f>Y17 &amp; "f,"</f>
-        <v>7.095606682564f,</v>
+        <f t="shared" si="28"/>
+        <v>4f,</v>
       </c>
       <c r="AO17" s="1" t="str">
-        <f>Z17 &amp; "f,"</f>
-        <v>8.32589494977925f,</v>
+        <f t="shared" si="28"/>
+        <v>7f,</v>
       </c>
       <c r="AP17" s="1" t="str">
-        <f>AA17 &amp; "f,"</f>
-        <v>6.60896018141239f,</v>
+        <f t="shared" si="28"/>
+        <v>10f,</v>
       </c>
     </row>
     <row r="18" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D18" s="2">
-        <f t="shared" ref="D18:I18" si="39">$B$2*D11+$B$3*C18</f>
-        <v>7.0956066825640018</v>
+        <f t="shared" ref="D18:I18" si="40">$B$2*D11+$B$3*C18</f>
+        <v>4</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="39"/>
-        <v>11.432585282679947</v>
+        <f t="shared" si="40"/>
+        <v>7</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="39"/>
-        <v>10.831846598343251</v>
+        <f t="shared" si="40"/>
+        <v>9</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="39"/>
-        <v>14.357597891259417</v>
+        <f t="shared" si="40"/>
+        <v>13</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="39"/>
-        <v>11.966126131191643</v>
+        <f t="shared" si="40"/>
+        <v>16</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="39"/>
-        <v>6.5335048676306382</v>
+        <f t="shared" si="40"/>
+        <v>16</v>
       </c>
       <c r="K18" s="11">
         <f>K14+$B$3*$B$3*K17</f>
-        <v>1.183973879289304</v>
+        <v>5</v>
       </c>
       <c r="L18" s="11">
-        <f t="shared" ref="L18:P18" si="40">L14+$B$3*$B$3*L17</f>
-        <v>2.1684503283686887</v>
+        <f t="shared" ref="L18:P18" si="41">L14+$B$3*$B$3*L17</f>
+        <v>5</v>
       </c>
       <c r="M18" s="11">
-        <f t="shared" si="40"/>
-        <v>2.3150994484406882</v>
+        <f t="shared" si="41"/>
+        <v>4</v>
       </c>
       <c r="N18" s="11">
-        <f t="shared" si="40"/>
-        <v>2.2520584547046161</v>
+        <f t="shared" si="41"/>
+        <v>6</v>
       </c>
       <c r="O18" s="11">
-        <f t="shared" si="40"/>
-        <v>2.7850348673613041</v>
+        <f t="shared" si="41"/>
+        <v>6</v>
       </c>
       <c r="P18" s="11">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="R18" s="4">
-        <f t="shared" ref="R18:S18" si="41">$B$2*K18+$B$3*Q18</f>
-        <v>2.0399869940154707</v>
+        <f t="shared" ref="R18:S18" si="42">$B$2*K18+$B$3*Q18</f>
+        <v>5</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="41"/>
-        <v>4.850072814511698</v>
+        <f t="shared" si="42"/>
+        <v>10</v>
       </c>
       <c r="T18" s="4">
-        <f t="shared" si="31"/>
-        <v>3.988916349663306</v>
+        <f t="shared" si="32"/>
+        <v>4</v>
       </c>
       <c r="U18" s="5">
-        <f t="shared" si="32"/>
-        <v>6.0582450443722191</v>
+        <f t="shared" si="33"/>
+        <v>10</v>
       </c>
       <c r="V18" s="4">
-        <f t="shared" si="33"/>
-        <v>4.7986150764635269</v>
+        <f t="shared" si="34"/>
+        <v>6</v>
       </c>
       <c r="W18" s="5">
-        <f t="shared" si="34"/>
-        <v>2.6200438317490859</v>
+        <f t="shared" si="35"/>
+        <v>6</v>
       </c>
       <c r="Y18" s="6">
         <f>S11+$B$3*$B$3*X18+$B$3*S16</f>
-        <v>11.432585282679945</v>
+        <v>7</v>
       </c>
       <c r="Z18" s="6">
         <f>U11+$B$3*$B$3*Y18+$B$3*U16</f>
-        <v>14.357597891259417</v>
+        <v>13</v>
       </c>
       <c r="AA18" s="6">
         <f>W11+$B$3*$B$3*Z18+$B$3*W16</f>
-        <v>6.5335048676306382</v>
+        <v>16</v>
       </c>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1" t="str">
-        <f t="shared" si="35"/>
-        <v>1.1839738792893f,</v>
+        <f t="shared" si="36"/>
+        <v>5f,</v>
       </c>
       <c r="AE18" s="1" t="str">
         <f t="shared" si="24"/>
-        <v>2.16845032836869f,</v>
+        <v>5f,</v>
       </c>
       <c r="AF18" s="1" t="str">
         <f t="shared" si="25"/>
-        <v>2.31509944844069f,</v>
+        <v>4f,</v>
       </c>
       <c r="AG18" s="1" t="str">
         <f t="shared" si="26"/>
-        <v>2.25205845470462f,</v>
+        <v>6f,</v>
       </c>
       <c r="AH18" s="1" t="str">
         <f t="shared" si="27"/>
-        <v>2.7850348673613f,</v>
+        <v>6f,</v>
       </c>
       <c r="AJ18" s="1" t="str">
-        <f t="shared" si="36"/>
-        <v>4.8500728145117f,</v>
+        <f t="shared" si="37"/>
+        <v>10f,</v>
       </c>
       <c r="AK18" s="1" t="str">
-        <f t="shared" si="37"/>
-        <v>6.05824504437222f,</v>
+        <f t="shared" si="38"/>
+        <v>10f,</v>
       </c>
       <c r="AL18" s="1" t="str">
-        <f t="shared" si="38"/>
-        <v>2.62004383174909f,</v>
+        <f t="shared" si="39"/>
+        <v>6f,</v>
       </c>
       <c r="AN18" s="1" t="str">
-        <f>Y18 &amp; "f,"</f>
-        <v>11.4325852826799f,</v>
+        <f t="shared" si="28"/>
+        <v>7f,</v>
       </c>
       <c r="AO18" s="1" t="str">
-        <f>Z18 &amp; "f,"</f>
-        <v>14.3575978912594f,</v>
+        <f t="shared" si="28"/>
+        <v>13f,</v>
       </c>
       <c r="AP18" s="1" t="str">
-        <f>AA18 &amp; "f,"</f>
-        <v>6.53350486763064f,</v>
+        <f t="shared" si="28"/>
+        <v>16f,</v>
       </c>
     </row>
     <row r="19" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D19" s="2">
-        <f t="shared" ref="D19:I19" si="42">$B$2*D12+$B$3*C19</f>
-        <v>6.842930248679945</v>
+        <f t="shared" ref="D19:I19" si="43">$B$2*D12+$B$3*C19</f>
+        <v>5</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="42"/>
-        <v>10.831846598343251</v>
+        <f t="shared" si="43"/>
+        <v>9</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="42"/>
-        <v>8.4201398912594154</v>
+        <f t="shared" si="43"/>
+        <v>11</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="42"/>
-        <v>12.176227048743588</v>
+        <f t="shared" si="43"/>
+        <v>16</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="42"/>
-        <v>11.870224183293946</v>
+        <f t="shared" si="43"/>
+        <v>20</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="42"/>
-        <v>6.4811424040784944</v>
+        <f t="shared" si="43"/>
+        <v>20</v>
       </c>
       <c r="Y19" s="6">
         <f>S12+$B$3*$B$3*X19+$B$3*$B$3*S16</f>
-        <v>10.831846598343251</v>
+        <v>9</v>
       </c>
       <c r="Z19" s="6">
         <f>U12+$B$3*$B$3*Y19+$B$3*$B$3*U16</f>
-        <v>12.176227048743586</v>
+        <v>16</v>
       </c>
       <c r="AA19" s="6">
         <f>W12+$B$3*$B$3*Z19+$B$3*$B$3*W16</f>
-        <v>6.4811424040784935</v>
+        <v>20</v>
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
       <c r="AN19" s="1" t="str">
-        <f>Y19 &amp; "f,"</f>
-        <v>10.8318465983433f,</v>
+        <f t="shared" si="28"/>
+        <v>9f,</v>
       </c>
       <c r="AO19" s="1" t="str">
-        <f>Z19 &amp; "f,"</f>
-        <v>12.1762270487436f,</v>
+        <f t="shared" si="28"/>
+        <v>16f,</v>
       </c>
       <c r="AP19" s="1" t="str">
-        <f>AA19 &amp; "f,"</f>
-        <v>6.48114240407849f,</v>
+        <f t="shared" si="28"/>
+        <v>20f,</v>
       </c>
     </row>
     <row r="20" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D20" s="2">
-        <f t="shared" ref="D20:I20" si="43">$B$2*D13+$B$3*C20</f>
-        <v>3.7362399157792501</v>
+        <f t="shared" ref="D20:I20" si="44">$B$2*D13+$B$3*C20</f>
+        <v>5</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="43"/>
-        <v>8.8829172426954166</v>
+        <f t="shared" si="44"/>
+        <v>10</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="43"/>
-        <v>12.155780414627642</v>
+        <f t="shared" si="44"/>
+        <v>14</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="43"/>
-        <v>13.743826651178001</v>
+        <f t="shared" si="44"/>
+        <v>20</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="43"/>
-        <v>16.292801652758442</v>
+        <f t="shared" si="44"/>
+        <v>26</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="43"/>
-        <v>8.8958697024061095</v>
+        <f t="shared" si="44"/>
+        <v>26</v>
       </c>
       <c r="Y20" s="6">
         <f>S13+$B$3*$B$3*X20+$B$3*S17</f>
-        <v>8.8829172426954148</v>
+        <v>10</v>
       </c>
       <c r="Z20" s="6">
         <f>U13+$B$3*$B$3*Y20+$B$3*U17</f>
-        <v>13.743826651178001</v>
+        <v>20</v>
       </c>
       <c r="AA20" s="6">
         <f>W13+$B$3*$B$3*Z20+$B$3*W17</f>
-        <v>8.8958697024061095</v>
+        <v>26</v>
       </c>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AN20" s="1" t="str">
-        <f>Y20 &amp; "f,"</f>
-        <v>8.88291724269541f,</v>
+        <f t="shared" si="28"/>
+        <v>10f,</v>
       </c>
       <c r="AO20" s="1" t="str">
-        <f>Z20 &amp; "f,"</f>
-        <v>13.743826651178f,</v>
+        <f t="shared" si="28"/>
+        <v>20f,</v>
       </c>
       <c r="AP20" s="1" t="str">
-        <f>AA20 &amp; "f,"</f>
-        <v>8.89586970240611f,</v>
+        <f t="shared" si="28"/>
+        <v>26f,</v>
       </c>
     </row>
     <row r="21" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D21" s="2">
-        <f t="shared" ref="D21:I21" si="44">$B$2*D14+$B$3*C21</f>
-        <v>2.0399869940154707</v>
+        <f t="shared" ref="D21:I21" si="45">$B$2*D14+$B$3*C21</f>
+        <v>5</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="44"/>
-        <v>4.8500728145116971</v>
+        <f t="shared" si="45"/>
+        <v>10</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="44"/>
-        <v>6.6370561063866926</v>
+        <f t="shared" si="45"/>
+        <v>14</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="44"/>
-        <v>7.5041293515431882</v>
+        <f t="shared" si="45"/>
+        <v>20</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="44"/>
-        <v>8.8958697024061077</v>
+        <f t="shared" si="45"/>
+        <v>26</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="44"/>
-        <v>4.8571448575137355</v>
+        <f t="shared" si="45"/>
+        <v>26</v>
       </c>
       <c r="Y21" s="6">
         <f>S14+$B$3*$B$3*X21+$B$3*$B$3*S17</f>
-        <v>4.8500728145116971</v>
+        <v>10</v>
       </c>
       <c r="Z21" s="6">
         <f>U14+$B$3*$B$3*Y21+$B$3*$B$3*U17</f>
-        <v>7.5041293515431882</v>
+        <v>20</v>
       </c>
       <c r="AA21" s="6">
         <f>W14+$B$3*$B$3*Z21+$B$3*$B$3*W17</f>
-        <v>4.8571448575137355</v>
+        <v>26</v>
       </c>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
@@ -1869,406 +1869,406 @@
     <row r="23" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K23" s="2">
         <f>K9+$B$3*K15</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" ref="L23:P23" si="45">L9+$B$3*L15</f>
+        <f t="shared" ref="L23:P23" si="46">L9+$B$3*L15</f>
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="45"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="46"/>
+        <v>1</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" si="45"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="46"/>
+        <v>1</v>
       </c>
       <c r="P23" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="R23" s="2">
-        <f t="shared" ref="R23:R28" si="46">$B$2*K23+$B$3*X16</f>
-        <v>2.9687290000000002</v>
+        <f t="shared" ref="R23:R28" si="47">$B$2*K23+$B$3*X16</f>
+        <v>1</v>
       </c>
       <c r="S23" s="2">
-        <f t="shared" ref="S23:S28" si="47">$B$2*L23+$B$3*R23</f>
-        <v>1.6209260340000002</v>
+        <f t="shared" ref="S23:S28" si="48">$B$2*L23+$B$3*R23</f>
+        <v>1</v>
       </c>
       <c r="T23" s="2">
-        <f t="shared" ref="T23:T28" si="48">$B$2*M23+$B$3*Y16</f>
-        <v>0.8850256145640002</v>
+        <f t="shared" ref="T23:T28" si="49">$B$2*M23+$B$3*Y16</f>
+        <v>1</v>
       </c>
       <c r="U23" s="2">
-        <f t="shared" ref="U23:U28" si="49">$B$2*N23+$B$3*T23</f>
-        <v>3.4519529855519444</v>
+        <f t="shared" ref="U23:U28" si="50">$B$2*N23+$B$3*T23</f>
+        <v>2</v>
       </c>
       <c r="V23" s="2">
-        <f t="shared" ref="V23:V28" si="50">$B$2*O23+$B$3*Z16</f>
-        <v>4.8534953301113619</v>
+        <f t="shared" ref="V23:V28" si="51">$B$2*O23+$B$3*Z16</f>
+        <v>3</v>
       </c>
       <c r="W23" s="2">
-        <f t="shared" ref="W23:W28" si="51">$B$2*P23+$B$3*V23</f>
-        <v>2.6500084502408039</v>
+        <f t="shared" ref="W23:W28" si="52">$B$2*P23+$B$3*V23</f>
+        <v>3</v>
       </c>
       <c r="AD23" s="1" t="str">
-        <f>R23 &amp; "f,"</f>
-        <v>2.968729f,</v>
+        <f t="shared" ref="AD23:AH27" si="53">R23 &amp; "f,"</f>
+        <v>1f,</v>
       </c>
       <c r="AE23" s="1" t="str">
-        <f>S23 &amp; "f,"</f>
-        <v>1.620926034f,</v>
+        <f t="shared" si="53"/>
+        <v>1f,</v>
       </c>
       <c r="AF23" s="1" t="str">
-        <f>T23 &amp; "f,"</f>
-        <v>0.885025614564f,</v>
+        <f t="shared" si="53"/>
+        <v>1f,</v>
       </c>
       <c r="AG23" s="1" t="str">
-        <f>U23 &amp; "f,"</f>
-        <v>3.45195298555194f,</v>
+        <f t="shared" si="53"/>
+        <v>2f,</v>
       </c>
       <c r="AH23" s="1" t="str">
-        <f>V23 &amp; "f,"</f>
-        <v>4.85349533011136f,</v>
+        <f t="shared" si="53"/>
+        <v>3f,</v>
       </c>
       <c r="AI23" s="2"/>
     </row>
     <row r="24" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K24" s="2">
         <f>K10+$B$3*$B$3*K15</f>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" ref="L24:P24" si="52">L10+$B$3*$B$3*L15</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="L24:P24" si="54">L10+$B$3*$B$3*L15</f>
+        <v>1</v>
       </c>
       <c r="M24" s="2">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="54"/>
+        <v>2</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="54"/>
+        <v>3</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="47"/>
+        <v>3</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="48"/>
+        <v>4</v>
+      </c>
+      <c r="T24" s="2">
+        <f t="shared" si="49"/>
+        <v>5</v>
+      </c>
+      <c r="U24" s="2">
+        <f t="shared" si="50"/>
+        <v>7</v>
+      </c>
+      <c r="V24" s="2">
+        <f t="shared" si="51"/>
+        <v>10</v>
+      </c>
+      <c r="W24" s="2">
         <f t="shared" si="52"/>
-        <v>1.7230000000000001</v>
-      </c>
-      <c r="N24" s="2">
-        <f t="shared" si="52"/>
-        <v>2.6637580000000001</v>
-      </c>
-      <c r="O24" s="2">
-        <f t="shared" si="52"/>
-        <v>4.3867580000000004</v>
-      </c>
-      <c r="P24" s="2">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="2">
-        <f t="shared" si="46"/>
-        <v>7.5583840340000013</v>
-      </c>
-      <c r="S24" s="2">
-        <f t="shared" si="47"/>
-        <v>7.0956066825640018</v>
-      </c>
-      <c r="T24" s="2">
-        <f t="shared" si="48"/>
-        <v>6.842930248679945</v>
-      </c>
-      <c r="U24" s="2">
-        <f t="shared" si="49"/>
-        <v>8.3258949497792507</v>
-      </c>
-      <c r="V24" s="2">
-        <f t="shared" si="50"/>
-        <v>12.104322676579471</v>
-      </c>
-      <c r="W24" s="2">
-        <f t="shared" si="51"/>
-        <v>6.6089601814123915</v>
+        <v>10</v>
       </c>
       <c r="AD24" s="1" t="str">
-        <f>R24 &amp; "f,"</f>
-        <v>7.558384034f,</v>
+        <f t="shared" si="53"/>
+        <v>3f,</v>
       </c>
       <c r="AE24" s="1" t="str">
-        <f>S24 &amp; "f,"</f>
-        <v>7.095606682564f,</v>
+        <f t="shared" si="53"/>
+        <v>4f,</v>
       </c>
       <c r="AF24" s="1" t="str">
-        <f>T24 &amp; "f,"</f>
-        <v>6.84293024867995f,</v>
+        <f t="shared" si="53"/>
+        <v>5f,</v>
       </c>
       <c r="AG24" s="1" t="str">
-        <f>U24 &amp; "f,"</f>
-        <v>8.32589494977925f,</v>
+        <f t="shared" si="53"/>
+        <v>7f,</v>
       </c>
       <c r="AH24" s="1" t="str">
-        <f>V24 &amp; "f,"</f>
-        <v>12.1043226765795f,</v>
+        <f t="shared" si="53"/>
+        <v>10f,</v>
       </c>
       <c r="AI24" s="2"/>
     </row>
     <row r="25" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K25" s="2">
         <f>K11+$B$3*K16</f>
-        <v>4.1181698680000007</v>
+        <v>4</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" ref="L25:P25" si="53">L11+$B$3*L16</f>
-        <v>4.3867580000000004</v>
+        <f t="shared" ref="L25:P25" si="55">L11+$B$3*L16</f>
+        <v>3</v>
       </c>
       <c r="M25" s="2">
+        <f t="shared" si="55"/>
+        <v>2</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="55"/>
+        <v>4</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="55"/>
+        <v>3</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="2">
+        <f t="shared" si="47"/>
+        <v>4</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="48"/>
+        <v>7</v>
+      </c>
+      <c r="T25" s="2">
+        <f t="shared" si="49"/>
+        <v>9</v>
+      </c>
+      <c r="U25" s="2">
+        <f t="shared" si="50"/>
+        <v>13</v>
+      </c>
+      <c r="V25" s="2">
+        <f t="shared" si="51"/>
+        <v>16</v>
+      </c>
+      <c r="W25" s="2">
+        <f t="shared" si="52"/>
+        <v>16</v>
+      </c>
+      <c r="AD25" s="1" t="str">
         <f t="shared" si="53"/>
-        <v>2.6637580000000001</v>
-      </c>
-      <c r="N25" s="2">
+        <v>4f,</v>
+      </c>
+      <c r="AE25" s="1" t="str">
         <f t="shared" si="53"/>
-        <v>4.9004118680000008</v>
-      </c>
-      <c r="O25" s="2">
+        <v>7f,</v>
+      </c>
+      <c r="AF25" s="1" t="str">
         <f t="shared" si="53"/>
-        <v>2.3951698680000004</v>
-      </c>
-      <c r="P25" s="2">
+        <v>9f,</v>
+      </c>
+      <c r="AG25" s="1" t="str">
         <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="2">
-        <f t="shared" si="46"/>
-        <v>7.0956066825640018</v>
-      </c>
-      <c r="S25" s="2">
-        <f t="shared" si="47"/>
-        <v>11.432585282679947</v>
-      </c>
-      <c r="T25" s="2">
-        <f t="shared" si="48"/>
-        <v>10.831846598343251</v>
-      </c>
-      <c r="U25" s="2">
-        <f t="shared" si="49"/>
-        <v>14.357597891259417</v>
-      </c>
-      <c r="V25" s="2">
-        <f t="shared" si="50"/>
-        <v>11.966126131191643</v>
-      </c>
-      <c r="W25" s="2">
-        <f t="shared" si="51"/>
-        <v>6.5335048676306382</v>
-      </c>
-      <c r="AD25" s="1" t="str">
-        <f>R25 &amp; "f,"</f>
-        <v>7.095606682564f,</v>
-      </c>
-      <c r="AE25" s="1" t="str">
-        <f>S25 &amp; "f,"</f>
-        <v>11.4325852826799f,</v>
-      </c>
-      <c r="AF25" s="1" t="str">
-        <f>T25 &amp; "f,"</f>
-        <v>10.8318465983433f,</v>
-      </c>
-      <c r="AG25" s="1" t="str">
-        <f>U25 &amp; "f,"</f>
-        <v>14.3575978912594f,</v>
+        <v>13f,</v>
       </c>
       <c r="AH25" s="1" t="str">
-        <f>V25 &amp; "f,"</f>
-        <v>11.9661261311916f,</v>
+        <f t="shared" si="53"/>
+        <v>16f,</v>
       </c>
       <c r="AI25" s="2"/>
     </row>
     <row r="26" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K26" s="2">
         <f>K12+$B$3*$B$3*K16</f>
-        <v>3.9715207479280004</v>
+        <v>5</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" ref="L26:P26" si="54">L12+$B$3*$B$3*L16</f>
-        <v>4.1181698680000007</v>
+        <f t="shared" ref="L26:P26" si="56">L12+$B$3*$B$3*L16</f>
+        <v>4</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="54"/>
-        <v>1.4544118680000002</v>
+        <f t="shared" si="56"/>
+        <v>2</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="54"/>
-        <v>4.3986248799280006</v>
+        <f t="shared" si="56"/>
+        <v>5</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="54"/>
-        <v>3.0307627479280006</v>
+        <f t="shared" si="56"/>
+        <v>4</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="46"/>
-        <v>6.842930248679945</v>
+        <f t="shared" si="47"/>
+        <v>5</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="47"/>
-        <v>10.831846598343251</v>
+        <f t="shared" si="48"/>
+        <v>9</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="48"/>
-        <v>8.4201398912594154</v>
+        <f t="shared" si="49"/>
+        <v>11</v>
       </c>
       <c r="U26" s="2">
-        <f t="shared" si="49"/>
-        <v>12.176227048743588</v>
+        <f t="shared" si="50"/>
+        <v>16</v>
       </c>
       <c r="V26" s="2">
-        <f t="shared" si="50"/>
-        <v>11.870224183293942</v>
+        <f t="shared" si="51"/>
+        <v>20</v>
       </c>
       <c r="W26" s="2">
-        <f t="shared" si="51"/>
-        <v>6.4811424040784926</v>
+        <f t="shared" si="52"/>
+        <v>20</v>
       </c>
       <c r="AD26" s="1" t="str">
-        <f>R26 &amp; "f,"</f>
-        <v>6.84293024867995f,</v>
+        <f t="shared" si="53"/>
+        <v>5f,</v>
       </c>
       <c r="AE26" s="1" t="str">
-        <f>S26 &amp; "f,"</f>
-        <v>10.8318465983433f,</v>
+        <f t="shared" si="53"/>
+        <v>9f,</v>
       </c>
       <c r="AF26" s="1" t="str">
-        <f>T26 &amp; "f,"</f>
-        <v>8.42013989125942f,</v>
+        <f t="shared" si="53"/>
+        <v>11f,</v>
       </c>
       <c r="AG26" s="1" t="str">
-        <f>U26 &amp; "f,"</f>
-        <v>12.1762270487436f,</v>
+        <f t="shared" si="53"/>
+        <v>16f,</v>
       </c>
       <c r="AH26" s="1" t="str">
-        <f>V26 &amp; "f,"</f>
-        <v>11.8702241832939f,</v>
+        <f t="shared" si="53"/>
+        <v>20f,</v>
       </c>
       <c r="AI26" s="2"/>
     </row>
     <row r="27" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K27" s="2">
         <f>K13+$B$3*K17</f>
-        <v>2.1684503283686882</v>
+        <v>5</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" ref="L27:P27" si="55">L13+$B$3*L17</f>
-        <v>3.9715207479280004</v>
+        <f t="shared" ref="L27:P27" si="57">L13+$B$3*L17</f>
+        <v>5</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="55"/>
-        <v>4.240108879928</v>
+        <f t="shared" si="57"/>
+        <v>4</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" si="55"/>
-        <v>4.1246491844406883</v>
+        <f t="shared" si="57"/>
+        <v>6</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="55"/>
-        <v>5.1007964603686888</v>
+        <f t="shared" si="57"/>
+        <v>6</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="R27" s="2">
-        <f t="shared" si="46"/>
-        <v>3.7362399157792501</v>
+        <f t="shared" si="47"/>
+        <v>5</v>
       </c>
       <c r="S27" s="2">
-        <f t="shared" si="47"/>
-        <v>8.8829172426954166</v>
+        <f t="shared" si="48"/>
+        <v>10</v>
       </c>
       <c r="T27" s="2">
-        <f t="shared" si="48"/>
-        <v>12.155780414627642</v>
+        <f t="shared" si="49"/>
+        <v>14</v>
       </c>
       <c r="U27" s="2">
-        <f t="shared" si="49"/>
-        <v>13.743826651178001</v>
+        <f t="shared" si="50"/>
+        <v>20</v>
       </c>
       <c r="V27" s="2">
-        <f t="shared" si="50"/>
-        <v>16.292801652758442</v>
+        <f t="shared" si="51"/>
+        <v>26</v>
       </c>
       <c r="W27" s="2">
-        <f t="shared" si="51"/>
-        <v>8.8958697024061095</v>
+        <f t="shared" si="52"/>
+        <v>26</v>
       </c>
       <c r="AD27" s="1" t="str">
-        <f>R27 &amp; "f,"</f>
-        <v>3.73623991577925f,</v>
+        <f t="shared" si="53"/>
+        <v>5f,</v>
       </c>
       <c r="AE27" s="1" t="str">
-        <f>S27 &amp; "f,"</f>
-        <v>8.88291724269542f,</v>
+        <f t="shared" si="53"/>
+        <v>10f,</v>
       </c>
       <c r="AF27" s="1" t="str">
-        <f>T27 &amp; "f,"</f>
-        <v>12.1557804146276f,</v>
+        <f t="shared" si="53"/>
+        <v>14f,</v>
       </c>
       <c r="AG27" s="1" t="str">
-        <f>U27 &amp; "f,"</f>
-        <v>13.743826651178f,</v>
+        <f t="shared" si="53"/>
+        <v>20f,</v>
       </c>
       <c r="AH27" s="1" t="str">
-        <f>V27 &amp; "f,"</f>
-        <v>16.2928016527584f,</v>
+        <f t="shared" si="53"/>
+        <v>26f,</v>
       </c>
       <c r="AI27" s="2"/>
     </row>
     <row r="28" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K28" s="2">
         <f>K14+$B$3*$B$3*K17</f>
-        <v>1.183973879289304</v>
+        <v>5</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" ref="L28:P28" si="56">L14+$B$3*$B$3*L17</f>
-        <v>2.1684503283686887</v>
+        <f t="shared" ref="L28:P28" si="58">L14+$B$3*$B$3*L17</f>
+        <v>5</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="56"/>
-        <v>2.3150994484406882</v>
+        <f t="shared" si="58"/>
+        <v>4</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="56"/>
-        <v>2.2520584547046161</v>
+        <f t="shared" si="58"/>
+        <v>6</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="56"/>
-        <v>2.7850348673613041</v>
+        <f t="shared" si="58"/>
+        <v>6</v>
       </c>
       <c r="P28" s="2">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="R28" s="2">
-        <f t="shared" si="46"/>
-        <v>2.0399869940154707</v>
+        <f t="shared" si="47"/>
+        <v>5</v>
       </c>
       <c r="S28" s="2">
-        <f t="shared" si="47"/>
-        <v>4.850072814511698</v>
+        <f t="shared" si="48"/>
+        <v>10</v>
       </c>
       <c r="T28" s="2">
-        <f t="shared" si="48"/>
-        <v>6.6370561063866926</v>
+        <f t="shared" si="49"/>
+        <v>14</v>
       </c>
       <c r="U28" s="2">
-        <f t="shared" si="49"/>
-        <v>7.5041293515431882</v>
+        <f t="shared" si="50"/>
+        <v>20</v>
       </c>
       <c r="V28" s="2">
-        <f t="shared" si="50"/>
-        <v>8.8958697024061077</v>
+        <f t="shared" si="51"/>
+        <v>26</v>
       </c>
       <c r="W28" s="2">
-        <f t="shared" si="51"/>
-        <v>4.8571448575137355</v>
+        <f t="shared" si="52"/>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="4:42" x14ac:dyDescent="0.2">
@@ -2277,23 +2277,23 @@
         <v>.</v>
       </c>
       <c r="L30" s="8" t="str">
-        <f t="shared" ref="L30:P30" si="57">IF(ABS(L23-E9)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="L30:P30" si="59">IF(ABS(L23-E9)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="M30" s="8" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>.</v>
       </c>
       <c r="N30" s="8" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>.</v>
       </c>
       <c r="O30" s="8" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>.</v>
       </c>
       <c r="P30" s="8" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>.</v>
       </c>
       <c r="Q30" s="7"/>
@@ -2302,535 +2302,535 @@
         <v>.</v>
       </c>
       <c r="S30" s="8" t="str">
-        <f t="shared" ref="S30:W30" si="58">IF(ABS(S23-E16)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="S30:W30" si="60">IF(ABS(S23-E16)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="T30" s="8" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>.</v>
       </c>
       <c r="U30" s="8" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>.</v>
       </c>
       <c r="V30" s="8" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>.</v>
       </c>
       <c r="W30" s="8" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>.</v>
       </c>
     </row>
     <row r="31" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K31" s="8" t="str">
-        <f t="shared" ref="K31:P31" si="59">IF(ABS(K24-D10)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K31:P31" si="61">IF(ABS(K24-D10)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L31" s="8" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>.</v>
       </c>
       <c r="M31" s="8" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>.</v>
       </c>
       <c r="N31" s="8" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>.</v>
       </c>
       <c r="O31" s="8" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>.</v>
       </c>
       <c r="P31" s="8" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>.</v>
       </c>
       <c r="Q31" s="7"/>
       <c r="R31" s="8" t="str">
-        <f t="shared" ref="R31:W31" si="60">IF(ABS(R24-D17)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R31:W31" si="62">IF(ABS(R24-D17)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S31" s="8" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>.</v>
       </c>
       <c r="T31" s="8" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>.</v>
       </c>
       <c r="U31" s="8" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>.</v>
       </c>
       <c r="V31" s="8" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>.</v>
       </c>
       <c r="W31" s="8" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>.</v>
       </c>
     </row>
     <row r="32" spans="4:42" x14ac:dyDescent="0.2">
       <c r="K32" s="8" t="str">
-        <f t="shared" ref="K32:P32" si="61">IF(ABS(K25-D11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K32:P32" si="63">IF(ABS(K25-D11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L32" s="8" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>.</v>
       </c>
       <c r="M32" s="8" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>.</v>
       </c>
       <c r="N32" s="8" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>.</v>
       </c>
       <c r="O32" s="8" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>.</v>
       </c>
       <c r="P32" s="8" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>.</v>
       </c>
       <c r="Q32" s="7"/>
       <c r="R32" s="8" t="str">
-        <f t="shared" ref="R32:W32" si="62">IF(ABS(R25-D18)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R32:W32" si="64">IF(ABS(R25-D18)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S32" s="8" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>.</v>
       </c>
       <c r="T32" s="8" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>.</v>
       </c>
       <c r="U32" s="8" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>.</v>
       </c>
       <c r="V32" s="8" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>.</v>
       </c>
       <c r="W32" s="8" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>.</v>
       </c>
     </row>
     <row r="33" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K33" s="8" t="str">
-        <f t="shared" ref="K33:P33" si="63">IF(ABS(K26-D12)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K33:P33" si="65">IF(ABS(K26-D12)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L33" s="8" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="M33" s="8" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="N33" s="8" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="O33" s="8" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="P33" s="8" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="Q33" s="7"/>
       <c r="R33" s="8" t="str">
-        <f t="shared" ref="R33:W33" si="64">IF(ABS(R26-D19)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R33:W33" si="66">IF(ABS(R26-D19)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S33" s="8" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="T33" s="8" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="U33" s="8" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="V33" s="8" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="W33" s="8" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
     </row>
     <row r="34" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K34" s="8" t="str">
-        <f t="shared" ref="K34:P34" si="65">IF(ABS(K27-D13)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K34:P34" si="67">IF(ABS(K27-D13)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L34" s="8" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="M34" s="8" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N34" s="8" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="O34" s="8" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="P34" s="8" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="8" t="str">
-        <f t="shared" ref="R34:W34" si="66">IF(ABS(R27-D20)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R34:W34" si="68">IF(ABS(R27-D20)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S34" s="8" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="T34" s="8" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="U34" s="8" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="V34" s="8" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="W34" s="8" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
     </row>
     <row r="35" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K35" s="8" t="str">
-        <f t="shared" ref="K35:P35" si="67">IF(ABS(K28-D14)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K35:P35" si="69">IF(ABS(K28-D14)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L35" s="8" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="M35" s="8" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="N35" s="8" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="O35" s="8" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P35" s="8" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="Q35" s="7"/>
       <c r="R35" s="8" t="str">
-        <f t="shared" ref="R35:W35" si="68">IF(ABS(R28-D21)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R35:W35" si="70">IF(ABS(R28-D21)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S35" s="8" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="T35" s="8" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="U35" s="8" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="V35" s="8" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="W35" s="8" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
     </row>
     <row r="38" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K38" s="9">
         <f>$B$2*D2</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="L38" s="9">
-        <f t="shared" ref="L38:P38" si="69">$B$2*E2</f>
+        <f t="shared" ref="L38:P38" si="71">$B$2*E2</f>
         <v>0</v>
       </c>
       <c r="M38" s="9">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="N38" s="9">
-        <f t="shared" si="69"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="71"/>
+        <v>1</v>
       </c>
       <c r="O38" s="9">
-        <f t="shared" si="69"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="71"/>
+        <v>1</v>
       </c>
       <c r="P38" s="9">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="R38" s="3">
         <f>$B$2*K38</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="S38" s="3">
-        <f t="shared" ref="S38:U38" si="70">$B$2*L38+$B$3*R38</f>
-        <v>1.6209260340000002</v>
+        <f t="shared" ref="S38:U38" si="72">$B$2*L38+$B$3*R38</f>
+        <v>1</v>
       </c>
       <c r="T38" s="3">
-        <f t="shared" si="70"/>
-        <v>0.8850256145640002</v>
+        <f t="shared" si="72"/>
+        <v>1</v>
       </c>
       <c r="U38" s="12">
-        <f t="shared" si="70"/>
-        <v>3.4519529855519444</v>
+        <f t="shared" si="72"/>
+        <v>2</v>
       </c>
       <c r="V38" s="3">
         <f>$B$2*O38</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="AD38" s="1" t="str">
         <f>K41 &amp; "f,"</f>
-        <v>3.971520747928f,</v>
+        <v>5f,</v>
       </c>
       <c r="AE38" s="1" t="str">
         <f>L41 &amp; "f,"</f>
-        <v>4.118169868f,</v>
+        <v>4f,</v>
       </c>
       <c r="AF38" s="1" t="str">
         <f>M41 &amp; "f,"</f>
-        <v>1.454411868f,</v>
+        <v>2f,</v>
       </c>
       <c r="AG38" s="1" t="str">
         <f>N41 &amp; "f,"</f>
-        <v>4.398624879928f,</v>
+        <v>5f,</v>
       </c>
       <c r="AH38" s="1" t="str">
         <f>O41 &amp; "f,"</f>
-        <v>3.030762747928f,</v>
+        <v>4f,</v>
       </c>
       <c r="AJ38" s="1" t="str">
         <f>U38 &amp; "f,"</f>
-        <v>3.45195298555194f,</v>
+        <v>2f,</v>
       </c>
       <c r="AK38" s="1" t="str">
         <f>V38 &amp; "f,"</f>
-        <v>2.968729f,</v>
+        <v>1f,</v>
       </c>
     </row>
     <row r="39" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K39" s="9">
         <f>$B$2*D3+$B$3*K38</f>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="L39" s="9">
-        <f t="shared" ref="L39:P39" si="71">$B$2*E3+$B$3*L38</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="L39:P39" si="73">$B$2*E3+$B$3*L38</f>
+        <v>1</v>
       </c>
       <c r="M39" s="9">
-        <f t="shared" si="71"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="73"/>
+        <v>1</v>
       </c>
       <c r="N39" s="9">
-        <f t="shared" si="71"/>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="73"/>
+        <v>2</v>
       </c>
       <c r="O39" s="9">
-        <f t="shared" si="71"/>
-        <v>4.3867580000000004</v>
+        <f t="shared" si="73"/>
+        <v>3</v>
       </c>
       <c r="P39" s="9">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="R39" s="3">
-        <f t="shared" ref="R39:R43" si="72">$B$2*K39</f>
-        <v>7.5583840340000013</v>
+        <f t="shared" ref="R39:R43" si="74">$B$2*K39</f>
+        <v>3</v>
       </c>
       <c r="S39" s="3">
-        <f t="shared" ref="S39:S43" si="73">$B$2*L39+$B$3*R39</f>
-        <v>7.0956066825640018</v>
+        <f t="shared" ref="S39:S43" si="75">$B$2*L39+$B$3*R39</f>
+        <v>4</v>
       </c>
       <c r="T39" s="3">
-        <f t="shared" ref="T39:T43" si="74">$B$2*M39+$B$3*S39</f>
-        <v>6.842930248679945</v>
+        <f t="shared" ref="T39:T43" si="76">$B$2*M39+$B$3*S39</f>
+        <v>5</v>
       </c>
       <c r="U39" s="12">
-        <f t="shared" ref="U39:U43" si="75">$B$2*N39+$B$3*T39</f>
-        <v>8.3258949497792507</v>
+        <f t="shared" ref="U39:U43" si="77">$B$2*N39+$B$3*T39</f>
+        <v>7</v>
       </c>
       <c r="V39" s="3">
-        <f t="shared" ref="V39:V43" si="76">$B$2*O39</f>
-        <v>7.5583840340000013</v>
+        <f t="shared" ref="V39:V43" si="78">$B$2*O39</f>
+        <v>3</v>
       </c>
       <c r="AD39" s="1" t="str">
         <f>K42 &amp; "f,"</f>
         <v>0f,</v>
       </c>
       <c r="AE39" s="1" t="str">
-        <f t="shared" ref="AE39:AH39" si="77">L42 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <f t="shared" ref="AE39:AH39" si="79">L42 &amp; "f,"</f>
+        <v>1f,</v>
       </c>
       <c r="AF39" s="1" t="str">
-        <f t="shared" si="77"/>
-        <v>3.446f,</v>
+        <f t="shared" si="79"/>
+        <v>2f,</v>
       </c>
       <c r="AG39" s="1" t="str">
-        <f t="shared" si="77"/>
-        <v>1.723f,</v>
+        <f t="shared" si="79"/>
+        <v>1f,</v>
       </c>
       <c r="AH39" s="1" t="str">
-        <f t="shared" si="77"/>
-        <v>3.446f,</v>
+        <f t="shared" si="79"/>
+        <v>2f,</v>
       </c>
       <c r="AJ39" s="1" t="str">
-        <f t="shared" ref="AJ39:AJ42" si="78">U39 &amp; "f,"</f>
-        <v>8.32589494977925f,</v>
+        <f t="shared" ref="AJ39:AJ42" si="80">U39 &amp; "f,"</f>
+        <v>7f,</v>
       </c>
       <c r="AK39" s="1" t="str">
-        <f t="shared" ref="AK39:AK42" si="79">V39 &amp; "f,"</f>
-        <v>7.558384034f,</v>
+        <f t="shared" ref="AK39:AK42" si="81">V39 &amp; "f,"</f>
+        <v>3f,</v>
       </c>
     </row>
     <row r="40" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K40" s="9">
         <f>$B$2*D4+$B$3*K39</f>
-        <v>4.1181698680000007</v>
+        <v>4</v>
       </c>
       <c r="L40" s="9">
-        <f t="shared" ref="L40:P40" si="80">$B$2*E4+$B$3*L39</f>
-        <v>4.3867580000000004</v>
+        <f t="shared" ref="L40:P40" si="82">$B$2*E4+$B$3*L39</f>
+        <v>3</v>
       </c>
       <c r="M40" s="9">
+        <f t="shared" si="82"/>
+        <v>2</v>
+      </c>
+      <c r="N40" s="9">
+        <f t="shared" si="82"/>
+        <v>4</v>
+      </c>
+      <c r="O40" s="9">
+        <f t="shared" si="82"/>
+        <v>3</v>
+      </c>
+      <c r="P40" s="9">
+        <f t="shared" si="82"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="3">
+        <f t="shared" si="74"/>
+        <v>4</v>
+      </c>
+      <c r="S40" s="3">
+        <f t="shared" si="75"/>
+        <v>7</v>
+      </c>
+      <c r="T40" s="3">
+        <f t="shared" si="76"/>
+        <v>9</v>
+      </c>
+      <c r="U40" s="12">
+        <f t="shared" si="77"/>
+        <v>13</v>
+      </c>
+      <c r="V40" s="3">
+        <f t="shared" si="78"/>
+        <v>3</v>
+      </c>
+      <c r="AJ40" s="1" t="str">
         <f t="shared" si="80"/>
-        <v>2.6637580000000001</v>
-      </c>
-      <c r="N40" s="9">
-        <f t="shared" si="80"/>
-        <v>4.9004118680000008</v>
-      </c>
-      <c r="O40" s="9">
-        <f t="shared" si="80"/>
-        <v>2.3951698680000004</v>
-      </c>
-      <c r="P40" s="9">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="R40" s="3">
-        <f t="shared" si="72"/>
-        <v>7.0956066825640018</v>
-      </c>
-      <c r="S40" s="3">
-        <f t="shared" si="73"/>
-        <v>11.432585282679947</v>
-      </c>
-      <c r="T40" s="3">
-        <f t="shared" si="74"/>
-        <v>10.831846598343251</v>
-      </c>
-      <c r="U40" s="12">
-        <f t="shared" si="75"/>
-        <v>14.357597891259417</v>
-      </c>
-      <c r="V40" s="3">
-        <f t="shared" si="76"/>
-        <v>4.1268776825640012</v>
-      </c>
-      <c r="AJ40" s="1" t="str">
-        <f t="shared" si="78"/>
-        <v>14.3575978912594f,</v>
+        <v>13f,</v>
       </c>
       <c r="AK40" s="1" t="str">
-        <f t="shared" si="79"/>
-        <v>4.126877682564f,</v>
+        <f t="shared" si="81"/>
+        <v>3f,</v>
       </c>
     </row>
     <row r="41" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K41" s="10">
         <f>$B$2*D5+$B$3*K40</f>
-        <v>3.9715207479280004</v>
+        <v>5</v>
       </c>
       <c r="L41" s="10">
-        <f t="shared" ref="L41:P41" si="81">$B$2*E5+$B$3*L40</f>
-        <v>4.1181698680000007</v>
+        <f t="shared" ref="L41:P41" si="83">$B$2*E5+$B$3*L40</f>
+        <v>4</v>
       </c>
       <c r="M41" s="10">
+        <f t="shared" si="83"/>
+        <v>2</v>
+      </c>
+      <c r="N41" s="10">
+        <f t="shared" si="83"/>
+        <v>5</v>
+      </c>
+      <c r="O41" s="10">
+        <f t="shared" si="83"/>
+        <v>4</v>
+      </c>
+      <c r="P41" s="10">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="R41" s="3">
+        <f t="shared" si="74"/>
+        <v>5</v>
+      </c>
+      <c r="S41" s="3">
+        <f t="shared" si="75"/>
+        <v>9</v>
+      </c>
+      <c r="T41" s="3">
+        <f t="shared" si="76"/>
+        <v>11</v>
+      </c>
+      <c r="U41" s="12">
+        <f t="shared" si="77"/>
+        <v>16</v>
+      </c>
+      <c r="V41" s="3">
+        <f t="shared" si="78"/>
+        <v>4</v>
+      </c>
+      <c r="AJ41" s="1" t="str">
+        <f t="shared" si="80"/>
+        <v>16f,</v>
+      </c>
+      <c r="AK41" s="1" t="str">
         <f t="shared" si="81"/>
-        <v>1.4544118680000002</v>
-      </c>
-      <c r="N41" s="10">
-        <f t="shared" si="81"/>
-        <v>4.3986248799280006</v>
-      </c>
-      <c r="O41" s="10">
-        <f t="shared" si="81"/>
-        <v>3.0307627479280006</v>
-      </c>
-      <c r="P41" s="10">
-        <f t="shared" si="81"/>
-        <v>0</v>
-      </c>
-      <c r="R41" s="3">
-        <f t="shared" si="72"/>
-        <v>6.842930248679945</v>
-      </c>
-      <c r="S41" s="3">
-        <f t="shared" si="73"/>
-        <v>10.831846598343251</v>
-      </c>
-      <c r="T41" s="3">
-        <f t="shared" si="74"/>
-        <v>8.4201398912594154</v>
-      </c>
-      <c r="U41" s="12">
-        <f t="shared" si="75"/>
-        <v>12.176227048743588</v>
-      </c>
-      <c r="V41" s="3">
-        <f t="shared" si="76"/>
-        <v>5.222004214679945</v>
-      </c>
-      <c r="AJ41" s="1" t="str">
-        <f t="shared" si="78"/>
-        <v>12.1762270487436f,</v>
-      </c>
-      <c r="AK41" s="1" t="str">
-        <f t="shared" si="79"/>
-        <v>5.22200421467995f,</v>
+        <v>4f,</v>
       </c>
     </row>
     <row r="42" spans="11:41" x14ac:dyDescent="0.2">
@@ -2839,304 +2839,304 @@
         <v>0</v>
       </c>
       <c r="L42" s="9">
-        <f t="shared" ref="L42:P42" si="82">$B$2*E6</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="L42:P42" si="84">$B$2*E6</f>
+        <v>1</v>
       </c>
       <c r="M42" s="9">
-        <f t="shared" si="82"/>
-        <v>3.4460000000000002</v>
+        <f t="shared" si="84"/>
+        <v>2</v>
       </c>
       <c r="N42" s="9">
-        <f t="shared" si="82"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="84"/>
+        <v>1</v>
       </c>
       <c r="O42" s="9">
-        <f t="shared" si="82"/>
-        <v>3.4460000000000002</v>
+        <f t="shared" si="84"/>
+        <v>2</v>
       </c>
       <c r="P42" s="9">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="R42" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" si="73"/>
-        <v>2.9687290000000002</v>
+        <f t="shared" si="75"/>
+        <v>1</v>
       </c>
       <c r="T42" s="3">
-        <f t="shared" si="74"/>
-        <v>7.5583840340000004</v>
+        <f t="shared" si="76"/>
+        <v>3</v>
       </c>
       <c r="U42" s="12">
-        <f t="shared" si="75"/>
-        <v>7.0956066825640001</v>
+        <f t="shared" si="77"/>
+        <v>4</v>
       </c>
       <c r="V42" s="3">
-        <f t="shared" si="76"/>
-        <v>5.9374580000000003</v>
+        <f t="shared" si="78"/>
+        <v>2</v>
       </c>
       <c r="AJ42" s="1" t="str">
-        <f t="shared" si="78"/>
-        <v>7.095606682564f,</v>
+        <f t="shared" si="80"/>
+        <v>4f,</v>
       </c>
       <c r="AK42" s="1" t="str">
-        <f t="shared" si="79"/>
-        <v>5.937458f,</v>
+        <f t="shared" si="81"/>
+        <v>2f,</v>
       </c>
     </row>
     <row r="43" spans="11:41" x14ac:dyDescent="0.2">
       <c r="R43" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="S43" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="T43" s="3">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="U43" s="12">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="V43" s="3">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="11:41" x14ac:dyDescent="0.2">
       <c r="R44" s="3">
-        <f t="shared" ref="R44:R45" si="83">$B$2*K44</f>
+        <f t="shared" ref="R44:R45" si="85">$B$2*K44</f>
         <v>0</v>
       </c>
       <c r="S44" s="3">
-        <f t="shared" ref="S44:S45" si="84">$B$2*L44+$B$3*R44</f>
+        <f t="shared" ref="S44:S45" si="86">$B$2*L44+$B$3*R44</f>
         <v>0</v>
       </c>
       <c r="T44" s="3">
-        <f t="shared" ref="T44:T45" si="85">$B$2*M44+$B$3*S44</f>
+        <f t="shared" ref="T44:T45" si="87">$B$2*M44+$B$3*S44</f>
         <v>0</v>
       </c>
       <c r="U44" s="12">
-        <f t="shared" ref="U44:U45" si="86">$B$2*N44+$B$3*T44</f>
+        <f t="shared" ref="U44:U45" si="88">$B$2*N44+$B$3*T44</f>
         <v>0</v>
       </c>
       <c r="V44" s="3">
-        <f t="shared" ref="V44:V45" si="87">$B$2*O44</f>
+        <f t="shared" ref="V44:V45" si="89">$B$2*O44</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="11:41" x14ac:dyDescent="0.2">
       <c r="R45" s="3">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="S45" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="T45" s="3">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="U45" s="12">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="V45" s="3">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K47" s="11">
         <f>K41+POWER($B$3,4)*K37</f>
-        <v>3.9715207479280004</v>
+        <v>5</v>
       </c>
       <c r="L47" s="11">
-        <f t="shared" ref="L47:P47" si="88">L41+POWER($B$3,4)*L37</f>
-        <v>4.1181698680000007</v>
+        <f t="shared" ref="L47:P47" si="90">L41+POWER($B$3,4)*L37</f>
+        <v>4</v>
       </c>
       <c r="M47" s="11">
-        <f t="shared" si="88"/>
-        <v>1.4544118680000002</v>
+        <f t="shared" si="90"/>
+        <v>2</v>
       </c>
       <c r="N47" s="11">
-        <f t="shared" si="88"/>
-        <v>4.3986248799280006</v>
+        <f t="shared" si="90"/>
+        <v>5</v>
       </c>
       <c r="O47" s="11">
-        <f t="shared" si="88"/>
-        <v>3.0307627479280006</v>
+        <f t="shared" si="90"/>
+        <v>4</v>
       </c>
       <c r="P47" s="11">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="R47" s="4">
         <f>$B$2*K47</f>
-        <v>6.842930248679945</v>
+        <v>5</v>
       </c>
       <c r="S47" s="4">
         <f>$B$2*L47+$B$3*R47</f>
-        <v>10.831846598343251</v>
+        <v>9</v>
       </c>
       <c r="T47" s="4">
         <f>$B$2*M47+$B$3*S47</f>
-        <v>8.4201398912594154</v>
+        <v>11</v>
       </c>
       <c r="U47" s="5">
         <f>$B$2*N47+$B$3*T47</f>
-        <v>12.176227048743588</v>
+        <v>16</v>
       </c>
       <c r="V47" s="4">
         <f>$B$2*O47</f>
-        <v>5.222004214679945</v>
+        <v>4</v>
       </c>
       <c r="Z47" s="14">
         <v>1</v>
       </c>
       <c r="AA47" s="6">
         <f>U38+POWER($B$3,$Z47)*U46+POWER($B$3,4)*0</f>
-        <v>3.4519529855519444</v>
+        <v>2</v>
       </c>
       <c r="AB47" s="6">
         <f>V38+POWER($B$3,$Z47)*V46+POWER($B$3,4)*AA47</f>
-        <v>3.2755149336000438</v>
+        <v>3</v>
       </c>
       <c r="AD47" s="14" t="str">
         <f>K47 &amp; "f,"</f>
-        <v>3.971520747928f,</v>
+        <v>5f,</v>
       </c>
       <c r="AE47" s="14" t="str">
-        <f t="shared" ref="AE47:AE48" si="89">L47 &amp; "f,"</f>
-        <v>4.118169868f,</v>
+        <f t="shared" ref="AE47:AE48" si="91">L47 &amp; "f,"</f>
+        <v>4f,</v>
       </c>
       <c r="AF47" s="14" t="str">
-        <f t="shared" ref="AF47:AF48" si="90">M47 &amp; "f,"</f>
-        <v>1.454411868f,</v>
+        <f t="shared" ref="AF47:AF48" si="92">M47 &amp; "f,"</f>
+        <v>2f,</v>
       </c>
       <c r="AG47" s="14" t="str">
-        <f t="shared" ref="AG47:AG48" si="91">N47 &amp; "f,"</f>
-        <v>4.398624879928f,</v>
+        <f t="shared" ref="AG47:AG48" si="93">N47 &amp; "f,"</f>
+        <v>5f,</v>
       </c>
       <c r="AH47" s="14" t="str">
-        <f t="shared" ref="AH47:AH48" si="92">O47 &amp; "f,"</f>
-        <v>3.030762747928f,</v>
+        <f t="shared" ref="AH47:AH48" si="94">O47 &amp; "f,"</f>
+        <v>4f,</v>
       </c>
       <c r="AJ47" s="14" t="str">
         <f>U47 &amp; "f,"</f>
-        <v>12.1762270487436f,</v>
+        <v>16f,</v>
       </c>
       <c r="AK47" s="14" t="str">
         <f>V47 &amp; "f,"</f>
-        <v>5.22200421467995f,</v>
+        <v>4f,</v>
       </c>
       <c r="AN47" s="14" t="str">
-        <f>AA47 &amp; ","</f>
-        <v>3.45195298555194,</v>
+        <f t="shared" ref="AN47:AO51" si="95">AA47 &amp; ","</f>
+        <v>2,</v>
       </c>
       <c r="AO47" s="14" t="str">
-        <f>AB47 &amp; ","</f>
-        <v>3.27551493360004,</v>
+        <f t="shared" si="95"/>
+        <v>3,</v>
       </c>
     </row>
     <row r="48" spans="11:41" x14ac:dyDescent="0.2">
       <c r="K48" s="11">
         <f>K42+POWER($B$3,4)*K47</f>
-        <v>0.35296155699821019</v>
+        <v>5</v>
       </c>
       <c r="L48" s="11">
-        <f t="shared" ref="L48:P48" si="93">L42+POWER($B$3,4)*L47</f>
-        <v>2.0889947261639601</v>
+        <f t="shared" ref="L48:P48" si="96">L42+POWER($B$3,4)*L47</f>
+        <v>5</v>
       </c>
       <c r="M48" s="11">
-        <f t="shared" si="93"/>
-        <v>3.5752581633153442</v>
+        <f t="shared" si="96"/>
+        <v>4</v>
       </c>
       <c r="N48" s="11">
-        <f t="shared" si="93"/>
-        <v>2.1139196463547214</v>
+        <f t="shared" si="96"/>
+        <v>6</v>
       </c>
       <c r="O48" s="11">
-        <f t="shared" si="93"/>
-        <v>3.7153534306622826</v>
+        <f t="shared" si="96"/>
+        <v>6</v>
       </c>
       <c r="P48" s="11">
-        <f t="shared" si="93"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="R48" s="4">
-        <f t="shared" ref="R48" si="94">$B$2*K48</f>
-        <v>0.60815276270791618</v>
+        <f t="shared" ref="R48" si="97">$B$2*K48</f>
+        <v>5</v>
       </c>
       <c r="S48" s="4">
-        <f t="shared" ref="S48:U48" si="95">$B$2*L48+$B$3*R48</f>
-        <v>3.9313893216190259</v>
+        <f t="shared" ref="S48:U48" si="98">$B$2*L48+$B$3*R48</f>
+        <v>10</v>
       </c>
       <c r="T48" s="4">
-        <f t="shared" si="95"/>
-        <v>8.3067083849963268</v>
+        <f t="shared" si="98"/>
+        <v>14</v>
       </c>
       <c r="U48" s="5">
-        <f t="shared" si="95"/>
-        <v>8.1777463288771806</v>
+        <f t="shared" si="98"/>
+        <v>20</v>
       </c>
       <c r="V48" s="4">
-        <f t="shared" ref="V48" si="96">$B$2*O48</f>
-        <v>6.4015539610311132</v>
+        <f t="shared" ref="V48" si="99">$B$2*O48</f>
+        <v>6</v>
       </c>
       <c r="Z48" s="14">
         <v>2</v>
       </c>
       <c r="AA48" s="6">
         <f>U39+POWER($B$3,Z48)*U46+POWER($B$3,4)*0</f>
-        <v>8.3258949497792507</v>
+        <v>7</v>
       </c>
       <c r="AB48" s="6">
         <f>V39+POWER($B$3,$Z48)*V46+POWER($B$3,4)*AA48</f>
-        <v>8.2983325402266885</v>
+        <v>10</v>
       </c>
       <c r="AD48" s="14" t="str">
-        <f t="shared" ref="AD48" si="97">K48 &amp; "f,"</f>
-        <v>0.35296155699821f,</v>
+        <f t="shared" ref="AD48" si="100">K48 &amp; "f,"</f>
+        <v>5f,</v>
       </c>
       <c r="AE48" s="14" t="str">
-        <f t="shared" si="89"/>
-        <v>2.08899472616396f,</v>
+        <f t="shared" si="91"/>
+        <v>5f,</v>
       </c>
       <c r="AF48" s="14" t="str">
-        <f t="shared" si="90"/>
-        <v>3.57525816331534f,</v>
+        <f t="shared" si="92"/>
+        <v>4f,</v>
       </c>
       <c r="AG48" s="14" t="str">
-        <f t="shared" si="91"/>
-        <v>2.11391964635472f,</v>
+        <f t="shared" si="93"/>
+        <v>6f,</v>
       </c>
       <c r="AH48" s="14" t="str">
-        <f t="shared" si="92"/>
-        <v>3.71535343066228f,</v>
+        <f t="shared" si="94"/>
+        <v>6f,</v>
       </c>
       <c r="AJ48" s="14" t="str">
         <f>U48 &amp; "f,"</f>
-        <v>8.17774632887718f,</v>
+        <v>20f,</v>
       </c>
       <c r="AK48" s="14" t="str">
         <f>V48 &amp; "f,"</f>
-        <v>6.40155396103111f,</v>
+        <v>6f,</v>
       </c>
       <c r="AN48" s="14" t="str">
-        <f>AA48 &amp; ","</f>
-        <v>8.32589494977925,</v>
+        <f t="shared" si="95"/>
+        <v>7,</v>
       </c>
       <c r="AO48" s="14" t="str">
-        <f>AB48 &amp; ","</f>
-        <v>8.29833254022669,</v>
+        <f t="shared" si="95"/>
+        <v>10,</v>
       </c>
     </row>
     <row r="49" spans="10:41" x14ac:dyDescent="0.2">
@@ -3145,19 +3145,19 @@
       </c>
       <c r="AA49" s="6">
         <f>U40+POWER($B$3,Z49)*U46+POWER($B$3,4)*0</f>
-        <v>14.357597891259417</v>
+        <v>13</v>
       </c>
       <c r="AB49" s="6">
         <f>V40+POWER($B$3,$Z49)*V46+POWER($B$3,4)*AA49</f>
-        <v>5.4028826257830502</v>
+        <v>16</v>
       </c>
       <c r="AN49" s="14" t="str">
-        <f>AA49 &amp; ","</f>
-        <v>14.3575978912594,</v>
+        <f t="shared" si="95"/>
+        <v>13,</v>
       </c>
       <c r="AO49" s="14" t="str">
-        <f>AB49 &amp; ","</f>
-        <v>5.40288262578305,</v>
+        <f t="shared" si="95"/>
+        <v>16,</v>
       </c>
     </row>
     <row r="50" spans="10:41" x14ac:dyDescent="0.2">
@@ -3166,19 +3166,19 @@
       </c>
       <c r="AA50" s="15">
         <f>U41+POWER($B$3,Z50)*U46+POWER($B$3,4)*0</f>
-        <v>12.176227048743588</v>
+        <v>16</v>
       </c>
       <c r="AB50" s="15">
         <f>V41+POWER($B$3,$Z50)*V46+POWER($B$3,4)*AA50</f>
-        <v>6.3041438609931237</v>
+        <v>20</v>
       </c>
       <c r="AN50" s="14" t="str">
-        <f>AA50 &amp; ","</f>
-        <v>12.1762270487436,</v>
+        <f t="shared" si="95"/>
+        <v>16,</v>
       </c>
       <c r="AO50" s="14" t="str">
-        <f>AB50 &amp; ","</f>
-        <v>6.30414386099312,</v>
+        <f t="shared" si="95"/>
+        <v>20,</v>
       </c>
     </row>
     <row r="51" spans="10:41" x14ac:dyDescent="0.2">
@@ -3187,82 +3187,82 @@
       </c>
       <c r="K51" s="2">
         <f>K38+POWER($B$3,$J51)*K$46</f>
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="L51" s="2">
-        <f t="shared" ref="L51:P51" si="98">L38+POWER($B$3,$J51)*L$46</f>
+        <f t="shared" ref="L51:O51" si="101">L38+POWER($B$3,$J51)*L$46</f>
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="98"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="N51" s="2">
-        <f t="shared" si="98"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="101"/>
+        <v>1</v>
       </c>
       <c r="O51" s="2">
-        <f t="shared" si="98"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="101"/>
+        <v>1</v>
       </c>
       <c r="R51" s="2">
         <f>$B$2*K51</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="S51" s="2">
         <f>$B$2*L51+$B$3*R51</f>
-        <v>1.6209260340000002</v>
+        <v>1</v>
       </c>
       <c r="T51" s="2">
         <f>$B$2*M51+$B$3*S51</f>
-        <v>0.8850256145640002</v>
+        <v>1</v>
       </c>
       <c r="U51" s="16">
         <f>$B$2*N51+$B$3*T51</f>
-        <v>3.4519529855519444</v>
+        <v>2</v>
       </c>
       <c r="V51" s="2">
         <f>$B$2*O51+$B$3*AA47</f>
-        <v>4.8534953301113619</v>
+        <v>3</v>
       </c>
       <c r="Z51" s="14">
         <v>1</v>
       </c>
       <c r="AA51" s="6">
         <f>U42+POWER($B$3,Z51)*U47+POWER($B$3,4)*0</f>
-        <v>13.743826651178001</v>
+        <v>20</v>
       </c>
       <c r="AB51" s="6">
         <f>V42+POWER($B$3,$Z51)*V47+POWER($B$3,4)*AA51</f>
-        <v>10.010129461282748</v>
+        <v>26</v>
       </c>
       <c r="AD51" s="14" t="str">
         <f>R51 &amp; ","</f>
-        <v>2.968729,</v>
+        <v>1,</v>
       </c>
       <c r="AE51" s="14" t="str">
-        <f t="shared" ref="AE51:AE55" si="99">S51 &amp; ","</f>
-        <v>1.620926034,</v>
+        <f t="shared" ref="AE51:AE55" si="102">S51 &amp; ","</f>
+        <v>1,</v>
       </c>
       <c r="AF51" s="14" t="str">
-        <f t="shared" ref="AF51:AF55" si="100">T51 &amp; ","</f>
-        <v>0.885025614564,</v>
+        <f t="shared" ref="AF51:AF55" si="103">T51 &amp; ","</f>
+        <v>1,</v>
       </c>
       <c r="AG51" s="14" t="str">
-        <f t="shared" ref="AG51:AG55" si="101">U51 &amp; ","</f>
-        <v>3.45195298555194,</v>
+        <f t="shared" ref="AG51:AG55" si="104">U51 &amp; ","</f>
+        <v>2,</v>
       </c>
       <c r="AH51" s="14" t="str">
-        <f t="shared" ref="AH51:AH55" si="102">V51 &amp; ","</f>
-        <v>4.85349533011136,</v>
+        <f t="shared" ref="AH51:AH55" si="105">V51 &amp; ","</f>
+        <v>3,</v>
       </c>
       <c r="AN51" s="14" t="str">
-        <f>AA51 &amp; ","</f>
-        <v>13.743826651178,</v>
+        <f t="shared" si="95"/>
+        <v>20,</v>
       </c>
       <c r="AO51" s="14" t="str">
-        <f>AB51 &amp; ","</f>
-        <v>10.0101294612827,</v>
+        <f t="shared" si="95"/>
+        <v>26,</v>
       </c>
     </row>
     <row r="52" spans="10:41" x14ac:dyDescent="0.2">
@@ -3271,63 +3271,63 @@
       </c>
       <c r="K52" s="2">
         <f>K39+POWER($B$3,$J52)*K$46</f>
-        <v>4.3867580000000004</v>
+        <v>3</v>
       </c>
       <c r="L52" s="2">
-        <f t="shared" ref="L52:P52" si="103">L39+POWER($B$3,$J52)*L$46</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="L52:O52" si="106">L39+POWER($B$3,$J52)*L$46</f>
+        <v>1</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" si="103"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="106"/>
+        <v>1</v>
       </c>
       <c r="N52" s="2">
-        <f t="shared" si="103"/>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="106"/>
+        <v>2</v>
       </c>
       <c r="O52" s="2">
-        <f t="shared" si="103"/>
-        <v>4.3867580000000004</v>
+        <f t="shared" si="106"/>
+        <v>3</v>
       </c>
       <c r="R52" s="2">
-        <f t="shared" ref="R52:R56" si="104">$B$2*K52</f>
-        <v>7.5583840340000013</v>
+        <f t="shared" ref="R52:R55" si="107">$B$2*K52</f>
+        <v>3</v>
       </c>
       <c r="S52" s="2">
-        <f t="shared" ref="S52:U52" si="105">$B$2*L52+$B$3*R52</f>
-        <v>7.0956066825640018</v>
+        <f t="shared" ref="S52:U52" si="108">$B$2*L52+$B$3*R52</f>
+        <v>4</v>
       </c>
       <c r="T52" s="2">
-        <f t="shared" si="105"/>
-        <v>6.842930248679945</v>
+        <f t="shared" si="108"/>
+        <v>5</v>
       </c>
       <c r="U52" s="16">
-        <f t="shared" si="105"/>
-        <v>8.3258949497792507</v>
+        <f t="shared" si="108"/>
+        <v>7</v>
       </c>
       <c r="V52" s="2">
         <f>$B$2*O52+$B$3*AA48</f>
-        <v>12.104322676579471</v>
+        <v>10</v>
       </c>
       <c r="AD52" s="14" t="str">
-        <f t="shared" ref="AD52:AD55" si="106">R52 &amp; ","</f>
-        <v>7.558384034,</v>
+        <f t="shared" ref="AD52:AD55" si="109">R52 &amp; ","</f>
+        <v>3,</v>
       </c>
       <c r="AE52" s="14" t="str">
-        <f t="shared" si="99"/>
-        <v>7.095606682564,</v>
+        <f t="shared" si="102"/>
+        <v>4,</v>
       </c>
       <c r="AF52" s="14" t="str">
-        <f t="shared" si="100"/>
-        <v>6.84293024867995,</v>
+        <f t="shared" si="103"/>
+        <v>5,</v>
       </c>
       <c r="AG52" s="14" t="str">
-        <f t="shared" si="101"/>
-        <v>8.32589494977925,</v>
+        <f t="shared" si="104"/>
+        <v>7,</v>
       </c>
       <c r="AH52" s="14" t="str">
-        <f t="shared" si="102"/>
-        <v>12.1043226765795,</v>
+        <f t="shared" si="105"/>
+        <v>10,</v>
       </c>
     </row>
     <row r="53" spans="10:41" x14ac:dyDescent="0.2">
@@ -3336,63 +3336,63 @@
       </c>
       <c r="K53" s="2">
         <f>K40+POWER($B$3,$J53)*K$46</f>
-        <v>4.1181698680000007</v>
+        <v>4</v>
       </c>
       <c r="L53" s="2">
-        <f t="shared" ref="L53:P53" si="107">L40+POWER($B$3,$J53)*L$46</f>
-        <v>4.3867580000000004</v>
+        <f t="shared" ref="L53:O53" si="110">L40+POWER($B$3,$J53)*L$46</f>
+        <v>3</v>
       </c>
       <c r="M53" s="2">
+        <f t="shared" si="110"/>
+        <v>2</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="110"/>
+        <v>4</v>
+      </c>
+      <c r="O53" s="2">
+        <f t="shared" si="110"/>
+        <v>3</v>
+      </c>
+      <c r="R53" s="2">
         <f t="shared" si="107"/>
-        <v>2.6637580000000001</v>
-      </c>
-      <c r="N53" s="2">
-        <f t="shared" si="107"/>
-        <v>4.9004118680000008</v>
-      </c>
-      <c r="O53" s="2">
-        <f t="shared" si="107"/>
-        <v>2.3951698680000004</v>
-      </c>
-      <c r="R53" s="2">
-        <f t="shared" si="104"/>
-        <v>7.0956066825640018</v>
+        <v>4</v>
       </c>
       <c r="S53" s="2">
-        <f t="shared" ref="S53:U53" si="108">$B$2*L53+$B$3*R53</f>
-        <v>11.432585282679947</v>
+        <f t="shared" ref="S53:U53" si="111">$B$2*L53+$B$3*R53</f>
+        <v>7</v>
       </c>
       <c r="T53" s="2">
-        <f t="shared" si="108"/>
-        <v>10.831846598343251</v>
+        <f t="shared" si="111"/>
+        <v>9</v>
       </c>
       <c r="U53" s="16">
-        <f t="shared" si="108"/>
-        <v>14.357597891259417</v>
+        <f t="shared" si="111"/>
+        <v>13</v>
       </c>
       <c r="V53" s="2">
         <f>$B$2*O53+$B$3*AA49</f>
-        <v>11.966126131191643</v>
+        <v>16</v>
       </c>
       <c r="AD53" s="14" t="str">
-        <f t="shared" si="106"/>
-        <v>7.095606682564,</v>
+        <f t="shared" si="109"/>
+        <v>4,</v>
       </c>
       <c r="AE53" s="14" t="str">
-        <f t="shared" si="99"/>
-        <v>11.4325852826799,</v>
+        <f t="shared" si="102"/>
+        <v>7,</v>
       </c>
       <c r="AF53" s="14" t="str">
-        <f t="shared" si="100"/>
-        <v>10.8318465983433,</v>
+        <f t="shared" si="103"/>
+        <v>9,</v>
       </c>
       <c r="AG53" s="14" t="str">
-        <f t="shared" si="101"/>
-        <v>14.3575978912594,</v>
+        <f t="shared" si="104"/>
+        <v>13,</v>
       </c>
       <c r="AH53" s="14" t="str">
-        <f t="shared" si="102"/>
-        <v>11.9661261311916,</v>
+        <f t="shared" si="105"/>
+        <v>16,</v>
       </c>
     </row>
     <row r="54" spans="10:41" x14ac:dyDescent="0.2">
@@ -3401,63 +3401,63 @@
       </c>
       <c r="K54" s="16">
         <f>K41+POWER($B$3,$J54)*K$46</f>
-        <v>3.9715207479280004</v>
+        <v>5</v>
       </c>
       <c r="L54" s="16">
-        <f t="shared" ref="L54:P54" si="109">L41+POWER($B$3,$J54)*L$46</f>
-        <v>4.1181698680000007</v>
+        <f t="shared" ref="L54:O54" si="112">L41+POWER($B$3,$J54)*L$46</f>
+        <v>4</v>
       </c>
       <c r="M54" s="16">
-        <f t="shared" si="109"/>
-        <v>1.4544118680000002</v>
+        <f t="shared" si="112"/>
+        <v>2</v>
       </c>
       <c r="N54" s="16">
-        <f t="shared" si="109"/>
-        <v>4.3986248799280006</v>
+        <f t="shared" si="112"/>
+        <v>5</v>
       </c>
       <c r="O54" s="16">
-        <f t="shared" si="109"/>
-        <v>3.0307627479280006</v>
+        <f t="shared" si="112"/>
+        <v>4</v>
       </c>
       <c r="R54" s="2">
-        <f t="shared" si="104"/>
-        <v>6.842930248679945</v>
+        <f t="shared" si="107"/>
+        <v>5</v>
       </c>
       <c r="S54" s="2">
-        <f t="shared" ref="S54:U54" si="110">$B$2*L54+$B$3*R54</f>
-        <v>10.831846598343251</v>
+        <f t="shared" ref="S54:U54" si="113">$B$2*L54+$B$3*R54</f>
+        <v>9</v>
       </c>
       <c r="T54" s="2">
-        <f t="shared" si="110"/>
-        <v>8.4201398912594154</v>
+        <f t="shared" si="113"/>
+        <v>11</v>
       </c>
       <c r="U54" s="16">
-        <f t="shared" si="110"/>
-        <v>12.176227048743588</v>
+        <f t="shared" si="113"/>
+        <v>16</v>
       </c>
       <c r="V54" s="2">
         <f>$B$2*O54+$B$3*AA50</f>
-        <v>11.870224183293946</v>
+        <v>20</v>
       </c>
       <c r="AD54" s="14" t="str">
-        <f t="shared" si="106"/>
-        <v>6.84293024867995,</v>
+        <f t="shared" si="109"/>
+        <v>5,</v>
       </c>
       <c r="AE54" s="14" t="str">
-        <f t="shared" si="99"/>
-        <v>10.8318465983433,</v>
+        <f t="shared" si="102"/>
+        <v>9,</v>
       </c>
       <c r="AF54" s="14" t="str">
-        <f t="shared" si="100"/>
-        <v>8.42013989125942,</v>
+        <f t="shared" si="103"/>
+        <v>11,</v>
       </c>
       <c r="AG54" s="14" t="str">
-        <f t="shared" si="101"/>
-        <v>12.1762270487436,</v>
+        <f t="shared" si="104"/>
+        <v>16,</v>
       </c>
       <c r="AH54" s="14" t="str">
-        <f t="shared" si="102"/>
-        <v>11.8702241832939,</v>
+        <f t="shared" si="105"/>
+        <v>20,</v>
       </c>
     </row>
     <row r="55" spans="10:41" x14ac:dyDescent="0.2">
@@ -3466,63 +3466,63 @@
       </c>
       <c r="K55" s="2">
         <f>K42+POWER($B$3,$J55)*K$47</f>
-        <v>2.1684503283686882</v>
+        <v>5</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" ref="L55:P55" si="111">L42+POWER($B$3,$J55)*L$47</f>
-        <v>3.9715207479280004</v>
+        <f t="shared" ref="L55:O55" si="114">L42+POWER($B$3,$J55)*L$47</f>
+        <v>5</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="111"/>
-        <v>4.240108879928</v>
+        <f t="shared" si="114"/>
+        <v>4</v>
       </c>
       <c r="N55" s="2">
-        <f t="shared" si="111"/>
-        <v>4.1246491844406883</v>
+        <f t="shared" si="114"/>
+        <v>6</v>
       </c>
       <c r="O55" s="2">
-        <f t="shared" si="111"/>
-        <v>5.1007964603686888</v>
+        <f t="shared" si="114"/>
+        <v>6</v>
       </c>
       <c r="R55" s="2">
-        <f t="shared" si="104"/>
-        <v>3.7362399157792501</v>
+        <f t="shared" si="107"/>
+        <v>5</v>
       </c>
       <c r="S55" s="2">
-        <f t="shared" ref="S55:U55" si="112">$B$2*L55+$B$3*R55</f>
-        <v>8.8829172426954166</v>
+        <f t="shared" ref="S55:U55" si="115">$B$2*L55+$B$3*R55</f>
+        <v>10</v>
       </c>
       <c r="T55" s="2">
-        <f t="shared" si="112"/>
-        <v>12.155780414627642</v>
+        <f t="shared" si="115"/>
+        <v>14</v>
       </c>
       <c r="U55" s="16">
-        <f t="shared" si="112"/>
-        <v>13.743826651178001</v>
+        <f t="shared" si="115"/>
+        <v>20</v>
       </c>
       <c r="V55" s="2">
         <f>$B$2*O55+$B$3*AA51</f>
-        <v>16.292801652758442</v>
+        <v>26</v>
       </c>
       <c r="AD55" s="14" t="str">
-        <f t="shared" si="106"/>
-        <v>3.73623991577925,</v>
+        <f t="shared" si="109"/>
+        <v>5,</v>
       </c>
       <c r="AE55" s="14" t="str">
-        <f t="shared" si="99"/>
-        <v>8.88291724269542,</v>
+        <f t="shared" si="102"/>
+        <v>10,</v>
       </c>
       <c r="AF55" s="14" t="str">
-        <f t="shared" si="100"/>
-        <v>12.1557804146276,</v>
+        <f t="shared" si="103"/>
+        <v>14,</v>
       </c>
       <c r="AG55" s="14" t="str">
-        <f t="shared" si="101"/>
-        <v>13.743826651178,</v>
+        <f t="shared" si="104"/>
+        <v>20,</v>
       </c>
       <c r="AH55" s="14" t="str">
-        <f t="shared" si="102"/>
-        <v>16.2928016527584,</v>
+        <f t="shared" si="105"/>
+        <v>26,</v>
       </c>
     </row>
     <row r="56" spans="10:41" x14ac:dyDescent="0.2">
@@ -3538,19 +3538,19 @@
         <v>.</v>
       </c>
       <c r="L58" s="8" t="str">
-        <f t="shared" ref="L58:P58" si="113">IF(ABS(L51-E9)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="L58:O58" si="116">IF(ABS(L51-E9)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="M58" s="8" t="str">
-        <f t="shared" si="113"/>
+        <f t="shared" si="116"/>
         <v>.</v>
       </c>
       <c r="N58" s="8" t="str">
-        <f t="shared" si="113"/>
+        <f t="shared" si="116"/>
         <v>.</v>
       </c>
       <c r="O58" s="8" t="str">
-        <f t="shared" si="113"/>
+        <f t="shared" si="116"/>
         <v>.</v>
       </c>
       <c r="P58" s="8"/>
@@ -3559,191 +3559,191 @@
         <v>.</v>
       </c>
       <c r="S58" s="8" t="str">
-        <f t="shared" ref="S58:W58" si="114">IF(ABS(S51-E16)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="S58:V58" si="117">IF(ABS(S51-E16)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="T58" s="8" t="str">
-        <f t="shared" si="114"/>
+        <f t="shared" si="117"/>
         <v>.</v>
       </c>
       <c r="U58" s="8" t="str">
-        <f t="shared" si="114"/>
+        <f t="shared" si="117"/>
         <v>.</v>
       </c>
       <c r="V58" s="8" t="str">
-        <f t="shared" si="114"/>
+        <f t="shared" si="117"/>
         <v>.</v>
       </c>
     </row>
     <row r="59" spans="10:41" x14ac:dyDescent="0.2">
       <c r="K59" s="8" t="str">
-        <f t="shared" ref="K59:P59" si="115">IF(ABS(K52-D10)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K59:O59" si="118">IF(ABS(K52-D10)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L59" s="8" t="str">
-        <f t="shared" si="115"/>
+        <f t="shared" si="118"/>
         <v>.</v>
       </c>
       <c r="M59" s="8" t="str">
-        <f t="shared" si="115"/>
+        <f t="shared" si="118"/>
         <v>.</v>
       </c>
       <c r="N59" s="8" t="str">
-        <f t="shared" si="115"/>
+        <f t="shared" si="118"/>
         <v>.</v>
       </c>
       <c r="O59" s="8" t="str">
-        <f t="shared" si="115"/>
+        <f t="shared" si="118"/>
         <v>.</v>
       </c>
       <c r="P59" s="8"/>
       <c r="R59" s="8" t="str">
-        <f t="shared" ref="R59:W59" si="116">IF(ABS(R52-D17)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R59:V59" si="119">IF(ABS(R52-D17)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S59" s="8" t="str">
-        <f t="shared" si="116"/>
+        <f t="shared" si="119"/>
         <v>.</v>
       </c>
       <c r="T59" s="8" t="str">
-        <f t="shared" si="116"/>
+        <f t="shared" si="119"/>
         <v>.</v>
       </c>
       <c r="U59" s="8" t="str">
-        <f t="shared" si="116"/>
+        <f t="shared" si="119"/>
         <v>.</v>
       </c>
       <c r="V59" s="8" t="str">
-        <f t="shared" si="116"/>
+        <f t="shared" si="119"/>
         <v>.</v>
       </c>
     </row>
     <row r="60" spans="10:41" x14ac:dyDescent="0.2">
       <c r="K60" s="8" t="str">
-        <f t="shared" ref="K60:P60" si="117">IF(ABS(K53-D11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K60:O60" si="120">IF(ABS(K53-D11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L60" s="8" t="str">
-        <f t="shared" si="117"/>
+        <f t="shared" si="120"/>
         <v>.</v>
       </c>
       <c r="M60" s="8" t="str">
-        <f t="shared" si="117"/>
+        <f t="shared" si="120"/>
         <v>.</v>
       </c>
       <c r="N60" s="8" t="str">
-        <f t="shared" si="117"/>
+        <f t="shared" si="120"/>
         <v>.</v>
       </c>
       <c r="O60" s="8" t="str">
-        <f t="shared" si="117"/>
+        <f t="shared" si="120"/>
         <v>.</v>
       </c>
       <c r="P60" s="8"/>
       <c r="R60" s="8" t="str">
-        <f t="shared" ref="R60:W60" si="118">IF(ABS(R53-D18)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R60:V60" si="121">IF(ABS(R53-D18)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S60" s="8" t="str">
-        <f t="shared" si="118"/>
+        <f t="shared" si="121"/>
         <v>.</v>
       </c>
       <c r="T60" s="8" t="str">
-        <f t="shared" si="118"/>
+        <f t="shared" si="121"/>
         <v>.</v>
       </c>
       <c r="U60" s="8" t="str">
-        <f t="shared" si="118"/>
+        <f t="shared" si="121"/>
         <v>.</v>
       </c>
       <c r="V60" s="8" t="str">
-        <f t="shared" si="118"/>
+        <f t="shared" si="121"/>
         <v>.</v>
       </c>
     </row>
     <row r="61" spans="10:41" x14ac:dyDescent="0.2">
       <c r="K61" s="8" t="str">
-        <f t="shared" ref="K61:P61" si="119">IF(ABS(K54-D12)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K61:O61" si="122">IF(ABS(K54-D12)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L61" s="8" t="str">
-        <f t="shared" si="119"/>
+        <f t="shared" si="122"/>
         <v>.</v>
       </c>
       <c r="M61" s="8" t="str">
-        <f t="shared" si="119"/>
+        <f t="shared" si="122"/>
         <v>.</v>
       </c>
       <c r="N61" s="8" t="str">
-        <f t="shared" si="119"/>
+        <f t="shared" si="122"/>
         <v>.</v>
       </c>
       <c r="O61" s="8" t="str">
-        <f t="shared" si="119"/>
+        <f t="shared" si="122"/>
         <v>.</v>
       </c>
       <c r="P61" s="8"/>
       <c r="R61" s="8" t="str">
-        <f t="shared" ref="R61:W61" si="120">IF(ABS(R54-D19)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R61:V61" si="123">IF(ABS(R54-D19)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S61" s="8" t="str">
-        <f t="shared" si="120"/>
+        <f t="shared" si="123"/>
         <v>.</v>
       </c>
       <c r="T61" s="8" t="str">
-        <f t="shared" si="120"/>
+        <f t="shared" si="123"/>
         <v>.</v>
       </c>
       <c r="U61" s="8" t="str">
-        <f t="shared" si="120"/>
+        <f t="shared" si="123"/>
         <v>.</v>
       </c>
       <c r="V61" s="8" t="str">
-        <f t="shared" si="120"/>
+        <f t="shared" si="123"/>
         <v>.</v>
       </c>
     </row>
     <row r="62" spans="10:41" x14ac:dyDescent="0.2">
       <c r="K62" s="8" t="str">
-        <f t="shared" ref="K62:P62" si="121">IF(ABS(K55-D13)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K62:O62" si="124">IF(ABS(K55-D13)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L62" s="8" t="str">
-        <f t="shared" si="121"/>
+        <f t="shared" si="124"/>
         <v>.</v>
       </c>
       <c r="M62" s="8" t="str">
-        <f t="shared" si="121"/>
+        <f t="shared" si="124"/>
         <v>.</v>
       </c>
       <c r="N62" s="8" t="str">
-        <f t="shared" si="121"/>
+        <f t="shared" si="124"/>
         <v>.</v>
       </c>
       <c r="O62" s="8" t="str">
-        <f t="shared" si="121"/>
+        <f t="shared" si="124"/>
         <v>.</v>
       </c>
       <c r="P62" s="8"/>
       <c r="R62" s="8" t="str">
-        <f t="shared" ref="R62:W62" si="122">IF(ABS(R55-D20)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R62:V62" si="125">IF(ABS(R55-D20)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S62" s="8" t="str">
-        <f t="shared" si="122"/>
+        <f t="shared" si="125"/>
         <v>.</v>
       </c>
       <c r="T62" s="8" t="str">
-        <f t="shared" si="122"/>
+        <f t="shared" si="125"/>
         <v>.</v>
       </c>
       <c r="U62" s="8" t="str">
-        <f t="shared" si="122"/>
+        <f t="shared" si="125"/>
         <v>.</v>
       </c>
       <c r="V62" s="8" t="str">
-        <f t="shared" si="122"/>
+        <f t="shared" si="125"/>
         <v>.</v>
       </c>
     </row>
@@ -4002,21 +4002,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4040,14 +4040,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCBCDE3-ADC9-411E-A5F5-6F7285261F5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32695E15-2B13-4DDA-A339-3037F2566A9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4063,4 +4055,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCBCDE3-ADC9-411E-A5F5-6F7285261F5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>